<commit_message>
Worked a bit on the Aquarium
</commit_message>
<xml_diff>
--- a/doc/Aquarium.xlsx
+++ b/doc/Aquarium.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="16275" windowHeight="10290" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="8595" windowHeight="8940"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="scratch" sheetId="1" r:id="rId1"/>
     <sheet name="radiation" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -46,13 +45,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.E+00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -81,14 +86,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -176,67 +182,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>7.8039393546240001</c:v>
+                  <c:v>10.418251392</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0597797646320002</c:v>
+                  <c:v>9.4247990685000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.3077176770048</c:v>
+                  <c:v>8.4207969184000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.5476973424880001</c:v>
+                  <c:v>7.4061705164999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.7796628158720003</c:v>
+                  <c:v>6.3808451760000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.003557955992</c:v>
+                  <c:v>5.3447459485</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2193264257280001</c:v>
+                  <c:v>4.2977976240000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.4269116920047997</c:v>
+                  <c:v>3.2399247308999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6262570257919999</c:v>
+                  <c:v>2.1710515359999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.81730550210399999</c:v>
+                  <c:v>1.0911020444999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.82571679741600001</c:v>
+                  <c:v>-1.1023311155</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-1.6599024029951999</c:v>
+                  <c:v>-2.2159680815999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-2.5026145255439998</c:v>
+                  <c:v>-3.3409879395000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-3.353911069824</c:v>
+                  <c:v>-4.4774679920000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-4.2138501365519998</c:v>
+                  <c:v>-5.6254858035000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-5.0824900224</c:v>
+                  <c:v>-6.7851191999999996</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-5.9598892199952003</c:v>
+                  <c:v>-7.9564462690999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-6.8461064179199997</c:v>
+                  <c:v>-9.1395453599999996</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-7.7412005007119999</c:v>
+                  <c:v>-10.3344950835</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-8.6452305488639993</c:v>
+                  <c:v>-11.541374312</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -252,67 +258,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>8.629656152039999</c:v>
+                  <c:v>11.5205825075</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.885496562048</c:v>
+                  <c:v>10.527130184000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.1334344744207998</c:v>
+                  <c:v>9.5231280339000008</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.3734141399039999</c:v>
+                  <c:v>8.5085016319999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.6053796132880001</c:v>
+                  <c:v>7.4831762915000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8292747534079998</c:v>
+                  <c:v>6.4470770640000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0450432231439999</c:v>
+                  <c:v>5.4001287395000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.2526284894208</c:v>
+                  <c:v>4.3422558463999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.4519738232079997</c:v>
+                  <c:v>3.2733826515</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6430222995199999</c:v>
+                  <c:v>2.1934331600000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.82571679741600001</c:v>
+                  <c:v>1.1023311155</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.83418560557919996</c:v>
+                  <c:v>-1.1136369661000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-1.676897728128</c:v>
+                  <c:v>-2.238656824</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-2.5281942724079998</c:v>
+                  <c:v>-3.3751368765</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-3.388133339136</c:v>
+                  <c:v>-4.523154688</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-4.2567732249840002</c:v>
+                  <c:v>-5.6827880845000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-5.1341724225791996</c:v>
+                  <c:v>-6.8541151535999996</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-6.020389620504</c:v>
+                  <c:v>-8.0372142444999994</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-6.9154837032960002</c:v>
+                  <c:v>-9.2321639680000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-7.8195137514479995</c:v>
+                  <c:v>-10.4390431965</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -328,67 +334,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>9.4638417576191998</c:v>
+                  <c:v>12.6342194736</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.7196821676271998</c:v>
+                  <c:v>11.6407671501</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.9676200799999997</c:v>
+                  <c:v>10.636765</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.2075997454831997</c:v>
+                  <c:v>9.6221385980999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.4395652188671999</c:v>
+                  <c:v>8.5968132575999991</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.6634603589871997</c:v>
+                  <c:v>7.5607140300999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.8792288287231997</c:v>
+                  <c:v>6.5137657056</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.0868140950000003</c:v>
+                  <c:v>5.4558928125000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2861594287872</c:v>
+                  <c:v>4.3870196176</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4772079050992</c:v>
+                  <c:v>3.3070701261000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.6599024029951999</c:v>
+                  <c:v>2.2159680815999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.83418560557919996</c:v>
+                  <c:v>1.1136369661000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.84271212254880001</c:v>
+                  <c:v>-1.1250198578999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1.6940086668287999</c:v>
+                  <c:v>-2.2614999104</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-2.5539477335567997</c:v>
+                  <c:v>-3.4095177218999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-3.4225876194047999</c:v>
+                  <c:v>-4.5691511183999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-4.2999868169999997</c:v>
+                  <c:v>-5.7404781874999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-5.1862040149248001</c:v>
+                  <c:v>-6.9235772783999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-6.0812980977167994</c:v>
+                  <c:v>-8.1185270019000004</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-6.9853281458687997</c:v>
+                  <c:v>-9.3254062304000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -404,67 +410,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>10.306553880168</c:v>
+                  <c:v>13.7592393315</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.562394290176</c:v>
+                  <c:v>12.765787008</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.8103322025487998</c:v>
+                  <c:v>11.7617848579</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0503118680319989</c:v>
+                  <c:v>10.747158455999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.282277341416</c:v>
+                  <c:v>9.7218331155000008</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.5061724815359998</c:v>
+                  <c:v>8.6857338879999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.7219409512719999</c:v>
+                  <c:v>7.6387855634999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9295262175487995</c:v>
+                  <c:v>6.5809126704000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.1288715513360001</c:v>
+                  <c:v>5.5120394755</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.3199200276480001</c:v>
+                  <c:v>4.4320899840000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5026145255439998</c:v>
+                  <c:v>3.3409879395000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.676897728128</c:v>
+                  <c:v>2.238656824</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.84271212254880001</c:v>
+                  <c:v>1.1250198578999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.85129654428000001</c:v>
+                  <c:v>-1.1364800525000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1.711235611008</c:v>
+                  <c:v>-2.284497864</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-2.5798754968559998</c:v>
+                  <c:v>-3.4441312604999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-3.4572746944512001</c:v>
+                  <c:v>-4.6154583296</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-4.343491892376</c:v>
+                  <c:v>-5.7985574204999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-5.2385859751680002</c:v>
+                  <c:v>-6.9935071439999996</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-6.1426160233199996</c:v>
+                  <c:v>-8.2003863725000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -480,67 +486,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>11.157850424448</c:v>
+                  <c:v>14.895719384</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.413690834456</c:v>
+                  <c:v>13.9022670605</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.6616287468288</c:v>
+                  <c:v>12.8982649104</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.9016084123119992</c:v>
+                  <c:v>11.883638508500001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.1335738856960003</c:v>
+                  <c:v>10.858313168</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.357469025816</c:v>
+                  <c:v>9.8222139404999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5732374955520001</c:v>
+                  <c:v>8.7752656160000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.7808227618287997</c:v>
+                  <c:v>7.7173927228999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.9801680956159995</c:v>
+                  <c:v>6.6485195279999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.1712165719279994</c:v>
+                  <c:v>5.5685700364999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.353911069824</c:v>
+                  <c:v>4.4774679920000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.5281942724079998</c:v>
+                  <c:v>3.3751368765</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.6940086668287999</c:v>
+                  <c:v>2.2614999104</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.85129654428000001</c:v>
+                  <c:v>1.1364800525000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.85993906672800002</c:v>
+                  <c:v>-1.1480178114999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-1.728578952576</c:v>
+                  <c:v>-2.3076512079999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-2.6059781501711998</c:v>
+                  <c:v>-3.4789782771</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-3.4921953480959997</c:v>
+                  <c:v>-4.6620773680000003</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-4.3872894308879999</c:v>
+                  <c:v>-5.8570270915</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-5.2913194790400002</c:v>
+                  <c:v>-7.0639063200000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -556,67 +562,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>12.017789491176</c:v>
+                  <c:v>16.0437371955</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.273629901184</c:v>
+                  <c:v>15.050284872000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.5215678135568</c:v>
+                  <c:v>14.046282721900001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.761547479039999</c:v>
+                  <c:v>13.03165632</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.9935129524240001</c:v>
+                  <c:v>12.0063309795</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.2174080925439998</c:v>
+                  <c:v>10.970231752</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.4331765622799999</c:v>
+                  <c:v>9.9232834274999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.6407618285567995</c:v>
+                  <c:v>8.8654105344000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.8401071623440002</c:v>
+                  <c:v>7.7965373395000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.0311556386560001</c:v>
+                  <c:v>6.7165878479999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.2138501365519998</c:v>
+                  <c:v>5.6254858035000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.388133339136</c:v>
+                  <c:v>4.523154688</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.5539477335567997</c:v>
+                  <c:v>3.4095177218999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.711235611008</c:v>
+                  <c:v>2.284497864</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.85993906672800002</c:v>
+                  <c:v>1.1480178114999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.868639885848</c:v>
+                  <c:v>-1.1596333965000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-1.7460390834432</c:v>
+                  <c:v>-2.3309604656</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2.6322562813679999</c:v>
+                  <c:v>-3.5140595564999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-3.5273503641599997</c:v>
+                  <c:v>-4.7090092800000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-4.4313804123119995</c:v>
+                  <c:v>-5.9158885085000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -632,79 +638,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>12.886429377023999</c:v>
+                  <c:v>17.203370591999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.142269787031999</c:v>
+                  <c:v>16.209918268500001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.390207699404799</c:v>
+                  <c:v>15.205916118399999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.630187364888</c:v>
+                  <c:v>14.1912897165</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.8621528382719994</c:v>
+                  <c:v>13.165964376</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.0860479783919992</c:v>
+                  <c:v>12.1298651485</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.3018164481279992</c:v>
+                  <c:v>11.082916824</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.5094017144047998</c:v>
+                  <c:v>10.025043930900001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.7087470481919995</c:v>
+                  <c:v>8.9561707360000007</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8997955245039995</c:v>
+                  <c:v>7.8762212444999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.0824900224</c:v>
+                  <c:v>6.7851191999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.2567732249840002</c:v>
+                  <c:v>5.6827880845000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.4225876194047999</c:v>
+                  <c:v>4.5691511183999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.5798754968559998</c:v>
+                  <c:v>3.4441312604999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.728578952576</c:v>
+                  <c:v>2.3076512079999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.868639885848</c:v>
+                  <c:v>1.1596333965000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.87739919759520002</c:v>
+                  <c:v>-1.1713270691</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-1.7636163955199999</c:v>
+                  <c:v>-2.35442616</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-2.6587104783119999</c:v>
+                  <c:v>-3.5493758835000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-3.5627405264639997</c:v>
+                  <c:v>-4.7562551119999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="81300096"/>
-        <c:axId val="112378240"/>
-        <c:axId val="127496640"/>
+        <c:axId val="142489088"/>
+        <c:axId val="142491008"/>
+        <c:axId val="140932864"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="81300096"/>
+        <c:axId val="142489088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,7 +745,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="112378240"/>
+        <c:crossAx val="142491008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -747,7 +753,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112378240"/>
+        <c:axId val="142491008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -784,12 +790,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81300096"/>
+        <c:crossAx val="142489088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="127496640"/>
+        <c:axId val="140932864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -824,7 +830,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="112378240"/>
+        <c:crossAx val="142491008"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -910,67 +916,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.34201243700799733</c:v>
+                  <c:v>0.52358607233333743</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2715768478367977</c:v>
+                  <c:v>0.42285464940000317</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2090437563007983</c:v>
+                  <c:v>0.33267305306666906</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15446891165439869</c:v>
+                  <c:v>0.2531157085333362</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10790825910719892</c:v>
+                  <c:v>0.18425730260000162</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.9417939823998687E-2</c:v>
+                  <c:v>0.12617278366666884</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.9054290924799062E-2</c:v>
+                  <c:v>7.8937361733334654E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6873845484799865E-2</c:v>
+                  <c:v>4.262650840000104E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.9333325343996464E-3</c:v>
+                  <c:v>1.7315956866667648E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-2.7103229408002028E-3</c:v>
+                  <c:v>3.0817019333337914E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.1121618252800225E-2</c:v>
+                  <c:v>8.1473690666662435E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.0712044668800287E-2</c:v>
+                  <c:v>2.7600588733332376E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.8828988054400178E-2</c:v>
+                  <c:v>5.8436700199999247E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.5530353171200844E-2</c:v>
+                  <c:v>0.10073300626666537</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.14087424073600108</c:v>
+                  <c:v>0.15456707133333136</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.19491894742080085</c:v>
+                  <c:v>0.22001672139999773</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.25772296585280152</c:v>
+                  <c:v>0.29716004406666396</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.32934498461440143</c:v>
+                  <c:v>0.3860753885333299</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.40984388824320206</c:v>
+                  <c:v>0.48684136559999658</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.49927875723200188</c:v>
+                  <c:v>0.59953684766666271</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -986,67 +992,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.33089081875519888</c:v>
+                  <c:v>0.51543870326667118</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26045522958399747</c:v>
+                  <c:v>0.41470728033333693</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19792213804799808</c:v>
+                  <c:v>0.32452568400000281</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14334729340159846</c:v>
+                  <c:v>0.24496833946666996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.6786640854398698E-2</c:v>
+                  <c:v>0.17610993353333537</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.829632157119935E-2</c:v>
+                  <c:v>0.11802541460000171</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.7932672671998837E-2</c:v>
+                  <c:v>7.0789992666668411E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.7522272319991963E-3</c:v>
+                  <c:v>3.447913933333524E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-8.1882857184001345E-3</c:v>
+                  <c:v>9.1685878000009602E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.3831941193600317E-2</c:v>
+                  <c:v>-5.0656671333326742E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-1.1121618252800225E-2</c:v>
+                  <c:v>-8.1473690666662435E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.9590426416000173E-2</c:v>
+                  <c:v>1.9453219666666355E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.7707369801600397E-2</c:v>
+                  <c:v>5.028933113333256E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.4408734918400175E-2</c:v>
+                  <c:v>9.2585637199999127E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.12975262248320085</c:v>
+                  <c:v>0.14641970226666512</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.18379732916800151</c:v>
+                  <c:v>0.21186935233333148</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.24660134760000041</c:v>
+                  <c:v>0.28901267499999772</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.3182233663616012</c:v>
+                  <c:v>0.37792801946666366</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.39872226999040183</c:v>
+                  <c:v>0.47869399653333033</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.48815713897920165</c:v>
+                  <c:v>0.59138947859999647</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1062,67 +1068,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.31130039233919859</c:v>
+                  <c:v>0.49598548360000372</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24086480316799808</c:v>
+                  <c:v>0.39525406066667124</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17833171163199779</c:v>
+                  <c:v>0.30507246433333712</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12375686698559818</c:v>
+                  <c:v>0.22551511980000427</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.7196214438398414E-2</c:v>
+                  <c:v>0.15665671386667057</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.8705895155199066E-2</c:v>
+                  <c:v>9.8572194933336021E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.3422462559994415E-3</c:v>
+                  <c:v>5.1336773000001834E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.3838199184001532E-2</c:v>
+                  <c:v>1.5025919666668663E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-2.7778712134400863E-2</c:v>
+                  <c:v>-1.0284631866665173E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-3.3422367609600379E-2</c:v>
+                  <c:v>-2.4518886799999251E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-3.0712044668800287E-2</c:v>
+                  <c:v>-2.7600588733332376E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1.9590426416000173E-2</c:v>
+                  <c:v>-1.9453219666666355E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.8116943385600224E-2</c:v>
+                  <c:v>3.0836111466666205E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.4818308502400335E-2</c:v>
+                  <c:v>7.313241753333255E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.11016219606720012</c:v>
+                  <c:v>0.12696648259999899</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.16420690275200078</c:v>
+                  <c:v>0.19241613266666491</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.22701092118400101</c:v>
+                  <c:v>0.26955945533333114</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.29863293994560092</c:v>
+                  <c:v>0.35847479979999797</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.37913184357440066</c:v>
+                  <c:v>0.45924077686666465</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.46856671256320137</c:v>
+                  <c:v>0.57193625893333078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1138,67 +1144,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.28318344895359715</c:v>
+                  <c:v>0.46514937213333774</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.21274785978239841</c:v>
+                  <c:v>0.36441794920000348</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15021476824639812</c:v>
+                  <c:v>0.27423635286667114</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.5639923599998511E-2</c:v>
+                  <c:v>0.19467900833333829</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9079271052797857E-2</c:v>
+                  <c:v>0.12582060240000281</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0588951769598509E-2</c:v>
+                  <c:v>6.7736083466670038E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.9774697129601115E-2</c:v>
+                  <c:v>2.0500661533335851E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-4.1955142569600312E-2</c:v>
+                  <c:v>-1.5810191799998208E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-5.5895655520001419E-2</c:v>
+                  <c:v>-4.1120743333331156E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-6.1539310995200935E-2</c:v>
+                  <c:v>-5.5354998266665234E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-5.8828988054400178E-2</c:v>
+                  <c:v>-5.8436700199999247E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-4.7707369801600397E-2</c:v>
+                  <c:v>-5.028933113333256E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-2.8116943385600224E-2</c:v>
+                  <c:v>-3.0836111466666205E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.6701365116800222E-2</c:v>
+                  <c:v>4.2296306066666345E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.2045252681600456E-2</c:v>
+                  <c:v>9.6130371133332559E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.13608995936640023</c:v>
+                  <c:v>0.16158002119999892</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.1988939777984009</c:v>
+                  <c:v>0.23872334386666516</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.27051599656000125</c:v>
+                  <c:v>0.3276386883333311</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.35101490018880099</c:v>
+                  <c:v>0.42840466539999777</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.44044976917760081</c:v>
+                  <c:v>0.54110014746666479</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1214,67 +1220,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.24648208383679737</c:v>
+                  <c:v>0.42285306606667206</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.17604649466559685</c:v>
+                  <c:v>0.3221216431333378</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11351340312959834</c:v>
+                  <c:v>0.23194004680000369</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8938558483198733E-2</c:v>
+                  <c:v>0.15238270226667083</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2377905935997191E-2</c:v>
+                  <c:v>8.3524296333337134E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.6112413347202157E-2</c:v>
+                  <c:v>2.543977740000436E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-5.6476062246401781E-2</c:v>
+                  <c:v>-2.1795644533330716E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-7.8656507686400978E-2</c:v>
+                  <c:v>-5.8106497866663886E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-9.2597020636800309E-2</c:v>
+                  <c:v>-8.3417049399997723E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-9.8240676112000713E-2</c:v>
+                  <c:v>-9.7651304333330913E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-9.5530353171200844E-2</c:v>
+                  <c:v>-0.10073300626666537</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-8.4408734918400175E-2</c:v>
+                  <c:v>-9.2585637199999127E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-6.4818308502400335E-2</c:v>
+                  <c:v>-7.313241753333255E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-3.6701365116800222E-2</c:v>
+                  <c:v>-4.2296306066666345E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.5343887564800234E-2</c:v>
+                  <c:v>5.3834065066666215E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.9388594249600448E-2</c:v>
+                  <c:v>0.11928371513333236</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.16219261268160023</c:v>
+                  <c:v>0.19642703779999904</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.23381463144320058</c:v>
+                  <c:v>0.28534238226666542</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.31431353507200122</c:v>
+                  <c:v>0.38610835933333121</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.40374840406080104</c:v>
+                  <c:v>0.49880384139999823</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1290,67 +1296,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.20113819627199625</c:v>
+                  <c:v>0.36901900100000518</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13070260710079751</c:v>
+                  <c:v>0.26828757806667092</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.8169515564797223E-2</c:v>
+                  <c:v>0.1781059817333368</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3594670918399387E-2</c:v>
+                  <c:v>9.8548637200003952E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.2965981628802155E-2</c:v>
+                  <c:v>2.9690231266672029E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-7.1456300912002391E-2</c:v>
+                  <c:v>-2.8394287666662521E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.10181994981120202</c:v>
+                  <c:v>-7.562970959999582E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.12400039525120121</c:v>
+                  <c:v>-0.11194056293333077</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.13794090820160143</c:v>
+                  <c:v>-0.1372511144666646</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.14358456367680095</c:v>
+                  <c:v>-0.15148536939999779</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.14087424073600108</c:v>
+                  <c:v>-0.15456707133333136</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.12975262248320085</c:v>
+                  <c:v>-0.14641970226666512</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.11016219606720012</c:v>
+                  <c:v>-0.12696648259999899</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-8.2045252681600456E-2</c:v>
+                  <c:v>-9.6130371133332559E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-4.5343887564800234E-2</c:v>
+                  <c:v>-5.3834065066666215E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.4044706684800214E-2</c:v>
+                  <c:v>6.5449650066666365E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.11684872511680044</c:v>
+                  <c:v>0.1425929727333326</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.18847074387840035</c:v>
+                  <c:v>0.23150831719999898</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.26896964750720054</c:v>
+                  <c:v>0.33227429426666522</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.3584045164960008</c:v>
+                  <c:v>0.44496977633333135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1366,79 +1372,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.14709348958719737</c:v>
+                  <c:v>0.30356935093334059</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.6657900415996849E-2</c:v>
+                  <c:v>0.20283792800000455</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4124808879998341E-2</c:v>
+                  <c:v>0.11265633166667222</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-4.0450035766403047E-2</c:v>
+                  <c:v>3.3098987133337587E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-8.7010688313601037E-2</c:v>
+                  <c:v>-3.5759418799996112E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.12550100759680127</c:v>
+                  <c:v>-9.3843937733328886E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.15586465649600179</c:v>
+                  <c:v>-0.14107935966666219</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.17804510193600187</c:v>
+                  <c:v>-0.17739021299999713</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.1919856148864012</c:v>
+                  <c:v>-0.20270076453333097</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.19762927036160072</c:v>
+                  <c:v>-0.21693501946666416</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.19491894742080085</c:v>
+                  <c:v>-0.22001672139999773</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.18379732916800151</c:v>
+                  <c:v>-0.21186935233333148</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.16420690275200078</c:v>
+                  <c:v>-0.19241613266666491</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.13608995936640023</c:v>
+                  <c:v>-0.16158002119999892</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-9.9388594249600448E-2</c:v>
+                  <c:v>-0.11928371513333236</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-5.4044706684800214E-2</c:v>
+                  <c:v>-6.5449650066666365E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.280401843200023E-2</c:v>
+                  <c:v>7.7143322666666236E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.13442603719360036</c:v>
+                  <c:v>0.16605866713333262</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.21492494082240032</c:v>
+                  <c:v>0.26682464419999929</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.30435980981120059</c:v>
+                  <c:v>0.37952012626666498</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="79714944"/>
-        <c:axId val="80938880"/>
-        <c:axId val="112388288"/>
+        <c:axId val="142534912"/>
+        <c:axId val="142934400"/>
+        <c:axId val="140945152"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="79714944"/>
+        <c:axId val="142534912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1473,7 +1479,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="80938880"/>
+        <c:crossAx val="142934400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1481,7 +1487,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80938880"/>
+        <c:axId val="142934400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -1520,12 +1526,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79714944"/>
+        <c:crossAx val="142534912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="112388288"/>
+        <c:axId val="140945152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1560,7 +1566,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="80938880"/>
+        <c:crossAx val="142934400"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -1928,106 +1934,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>32.450000000000003</v>
+      </c>
       <c r="B1">
-        <v>2618</v>
+        <v>31.36</v>
       </c>
       <c r="C1" s="1">
-        <f>1/B1</f>
-        <v>3.8197097020626432E-4</v>
+        <v>1.0940000000000001</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2184</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A1/A2</f>
+        <v>1.4858058608058609E-2</v>
+      </c>
+      <c r="B3">
+        <f>B1/A2</f>
+        <v>1.4358974358974359E-2</v>
+      </c>
+      <c r="C3" s="1">
+        <f>C1/A2</f>
+        <v>5.0091575091575091E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>10.37</v>
       </c>
-      <c r="C2" s="1">
-        <f>B2/B1</f>
-        <v>3.9610389610389611E-3</v>
-      </c>
-      <c r="D2" s="1">
-        <f>C2/B3</f>
-        <v>1.0915561510799606E-7</v>
+      <c r="B6">
+        <v>45.57</v>
+      </c>
+      <c r="C6">
+        <v>31.36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>36288</v>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>48384</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>33.869999999999997</v>
-      </c>
-      <c r="C4" s="1">
-        <f>B4/B3</f>
-        <v>9.3336640211640206E-4</v>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>A6/A7</f>
+        <v>2.1432705026455025E-4</v>
+      </c>
+      <c r="B8">
+        <f>B6/A7</f>
+        <v>9.4184027777777777E-4</v>
+      </c>
+      <c r="C8">
+        <f>C6/A7</f>
+        <v>6.4814814814814813E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>23.5</v>
-      </c>
-      <c r="C5" s="1">
-        <f>B5/B3</f>
-        <v>6.4759700176366839E-4</v>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>2.14E-4</v>
+      </c>
+      <c r="B10" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C10" s="1">
+        <f>A10*B10</f>
+        <v>8.5600000000000004E-7</v>
+      </c>
+      <c r="D10" s="4">
+        <v>3.8200000000000002E-4</v>
+      </c>
+      <c r="E10" s="1">
+        <f>B10*D10</f>
+        <v>1.528E-6</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1.15E-2</v>
+      </c>
+      <c r="G10" s="1">
+        <f>E10*F10</f>
+        <v>1.7572E-8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>1440</v>
-      </c>
-      <c r="C6">
-        <v>0.6</v>
-      </c>
-      <c r="D6">
-        <f>PRODUCT(A6:C6)</f>
-        <v>2592</v>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>6.4800000000000003E-4</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1.14E-2</v>
+      </c>
+      <c r="C11" s="1">
+        <f>A11*B11</f>
+        <v>7.3872000000000002E-6</v>
+      </c>
+      <c r="D11" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E11" s="1">
+        <f>B11*D11</f>
+        <v>5.7000000000000005E-6</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G11" s="1">
+        <f>E11*F11</f>
+        <v>2.2800000000000002E-8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2.6</v>
-      </c>
-      <c r="B7">
-        <v>840</v>
-      </c>
-      <c r="C7">
-        <f>A7*B7</f>
-        <v>2184</v>
-      </c>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0.2</v>
-      </c>
-      <c r="B8">
-        <v>5.7599999999999998E-2</v>
-      </c>
-      <c r="C8">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="D8">
-        <f>A8*B8/C8</f>
-        <v>3.8400000000000003</v>
-      </c>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <f>B2+B5+D8</f>
-        <v>37.71</v>
-      </c>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2039,8 +2084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2065,1354 +2110,1354 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
-        <v>8.1647999999999998E-9</v>
+        <v>1.09E-8</v>
       </c>
       <c r="R1" t="s">
         <v>5</v>
       </c>
       <c r="S1">
         <f>AVERAGE(J5:P25) - 0.02</f>
-        <v>0.81459517916319979</v>
+        <v>1.0941837464333337</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="J2" s="3" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="J2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="R2" s="3" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="R2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Z2" s="3" t="s">
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Z2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
     </row>
-    <row r="3" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="J3" s="5" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="J3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="R3" s="5" t="s">
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="R3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Z3" s="5" t="s">
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Z3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
-      <c r="AE3" s="5"/>
-      <c r="AF3" s="5"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
     </row>
-    <row r="4" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>20</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>21</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>22</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>23</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>24</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>25</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>26</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>20</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>21</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>22</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="3">
         <v>23</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>24</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="3">
         <v>25</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="3">
         <v>26</v>
       </c>
-      <c r="R4" s="4">
+      <c r="R4" s="3">
         <v>20</v>
       </c>
-      <c r="S4" s="4">
+      <c r="S4" s="3">
         <v>21</v>
       </c>
-      <c r="T4" s="4">
+      <c r="T4" s="3">
         <v>22</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U4" s="3">
         <v>23</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4" s="3">
         <v>24</v>
       </c>
-      <c r="W4" s="4">
+      <c r="W4" s="3">
         <v>25</v>
       </c>
-      <c r="X4" s="4">
+      <c r="X4" s="3">
         <v>26</v>
       </c>
-      <c r="Z4" s="4">
+      <c r="Z4" s="3">
         <v>20</v>
       </c>
-      <c r="AA4" s="4">
+      <c r="AA4" s="3">
         <v>21</v>
       </c>
-      <c r="AB4" s="4">
+      <c r="AB4" s="3">
         <v>22</v>
       </c>
-      <c r="AC4" s="4">
+      <c r="AC4" s="3">
         <v>23</v>
       </c>
-      <c r="AD4" s="4">
+      <c r="AD4" s="3">
         <v>24</v>
       </c>
-      <c r="AE4" s="4">
+      <c r="AE4" s="3">
         <v>25</v>
       </c>
-      <c r="AF4" s="4">
+      <c r="AF4" s="3">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>10</v>
       </c>
       <c r="B5">
         <f xml:space="preserve"> $A$1 * ( (B$4 + 273)^4 - ($A5 + 273)^4)</f>
-        <v>7.8039393546240001</v>
+        <v>10.418251392</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:H20" si="0" xml:space="preserve"> $A$1 * ( (C$4 + 273)^4 - ($A5 + 273)^4)</f>
-        <v>8.629656152039999</v>
+        <v>11.5205825075</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>9.4638417576191998</v>
+        <v>12.6342194736</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>10.306553880168</v>
+        <v>13.7592393315</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>11.157850424448</v>
+        <v>14.895719384</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>12.017789491176</v>
+        <v>16.0437371955</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>12.886429377023999</v>
+        <v>17.203370591999999</v>
       </c>
       <c r="J5">
         <f xml:space="preserve"> $A$1 * ( (J$4 + 273)^2 + ($A5 + 273)^2) *  ( (J$4 + 273) + ($A5 + 273))</f>
-        <v>0.78039393546239988</v>
+        <v>1.0418251392</v>
       </c>
       <c r="K5">
         <f t="shared" ref="K5:P5" si="1" xml:space="preserve"> $A$1 * ( (K$4 + 273)^2 + ($A5 + 273)^2) *  ( (K$4 + 273) + ($A5 + 273))</f>
-        <v>0.78451419564000002</v>
+        <v>1.0473256824999999</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>0.78865347980159994</v>
+        <v>1.0528516228</v>
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
-        <v>0.79281183693599999</v>
+        <v>1.0584030254999999</v>
       </c>
       <c r="N5">
         <f t="shared" si="1"/>
-        <v>0.79698931603199996</v>
+        <v>1.0639799560000001</v>
       </c>
       <c r="O5">
         <f t="shared" si="1"/>
-        <v>0.80118596607839998</v>
+        <v>1.0695824797</v>
       </c>
       <c r="P5">
         <f t="shared" si="1"/>
-        <v>0.80540183606400007</v>
+        <v>1.0752106619999999</v>
       </c>
       <c r="R5">
         <f xml:space="preserve"> $S$1 *  ( R$4 - $A5)</f>
-        <v>8.1459517916319975</v>
+        <v>10.941837464333338</v>
       </c>
       <c r="S5">
         <f t="shared" ref="S5:X5" si="2" xml:space="preserve"> $S$1 *  ( S$4 - $A5)</f>
-        <v>8.9605469707951979</v>
+        <v>12.036021210766672</v>
       </c>
       <c r="T5">
         <f t="shared" si="2"/>
-        <v>9.7751421499583984</v>
+        <v>13.130204957200004</v>
       </c>
       <c r="U5">
         <f t="shared" si="2"/>
-        <v>10.589737329121597</v>
+        <v>14.224388703633338</v>
       </c>
       <c r="V5">
         <f t="shared" si="2"/>
-        <v>11.404332508284797</v>
+        <v>15.318572450066672</v>
       </c>
       <c r="W5">
         <f t="shared" si="2"/>
-        <v>12.218927687447996</v>
+        <v>16.412756196500006</v>
       </c>
       <c r="X5">
         <f t="shared" si="2"/>
-        <v>13.033522866611197</v>
+        <v>17.506939942933339</v>
       </c>
       <c r="Z5">
         <f>R5-B5</f>
-        <v>0.34201243700799733</v>
+        <v>0.52358607233333743</v>
       </c>
       <c r="AA5">
         <f t="shared" ref="AA5:AF20" si="3">S5-C5</f>
-        <v>0.33089081875519888</v>
+        <v>0.51543870326667118</v>
       </c>
       <c r="AB5">
         <f t="shared" si="3"/>
-        <v>0.31130039233919859</v>
+        <v>0.49598548360000372</v>
       </c>
       <c r="AC5">
         <f t="shared" si="3"/>
-        <v>0.28318344895359715</v>
+        <v>0.46514937213333774</v>
       </c>
       <c r="AD5">
         <f t="shared" si="3"/>
-        <v>0.24648208383679737</v>
+        <v>0.42285306606667206</v>
       </c>
       <c r="AE5">
         <f t="shared" si="3"/>
-        <v>0.20113819627199625</v>
+        <v>0.36901900100000518</v>
       </c>
       <c r="AF5">
         <f t="shared" si="3"/>
-        <v>0.14709348958719737</v>
+        <v>0.30356935093334059</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>11</v>
       </c>
       <c r="B6">
         <f t="shared" ref="B6:H25" si="4" xml:space="preserve"> $A$1 * ( (B$4 + 273)^4 - ($A6 + 273)^4)</f>
-        <v>7.0597797646320002</v>
+        <v>9.4247990685000005</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>7.885496562048</v>
+        <v>10.527130184000001</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>8.7196821676271998</v>
+        <v>11.6407671501</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>9.562394290176</v>
+        <v>12.765787008</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>10.413690834456</v>
+        <v>13.9022670605</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>11.273629901184</v>
+        <v>15.050284872000001</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>12.142269787031999</v>
+        <v>16.209918268500001</v>
       </c>
       <c r="J6">
-        <f t="shared" ref="J6:X25" si="5" xml:space="preserve"> $A$1 * ( (J$4 + 273)^2 + ($A6 + 273)^2) *  ( (J$4 + 273) + ($A6 + 273))</f>
-        <v>0.784419973848</v>
+        <f t="shared" ref="J6:P25" si="5" xml:space="preserve"> $A$1 * ( (J$4 + 273)^2 + ($A6 + 273)^2) *  ( (J$4 + 273) + ($A6 + 273))</f>
+        <v>1.0471998965</v>
       </c>
       <c r="K6">
         <f t="shared" si="5"/>
-        <v>0.7885496562048</v>
+        <v>1.0527130184</v>
       </c>
       <c r="L6">
         <f t="shared" si="5"/>
-        <v>0.7926983788752</v>
+        <v>1.0582515591000001</v>
       </c>
       <c r="M6">
         <f t="shared" si="5"/>
-        <v>0.79686619084800003</v>
+        <v>1.0638155839999999</v>
       </c>
       <c r="N6">
         <f t="shared" si="5"/>
-        <v>0.80105314111199999</v>
+        <v>1.0694051585</v>
       </c>
       <c r="O6">
         <f t="shared" si="5"/>
-        <v>0.805259278656</v>
+        <v>1.075020348</v>
       </c>
       <c r="P6">
         <f t="shared" si="5"/>
-        <v>0.80948465246879997</v>
+        <v>1.0806612179000001</v>
       </c>
       <c r="R6">
-        <f t="shared" ref="R6:AF25" si="6" xml:space="preserve"> $S$1 *  ( R$4 - $A6)</f>
-        <v>7.3313566124687979</v>
+        <f t="shared" ref="R6:X25" si="6" xml:space="preserve"> $S$1 *  ( R$4 - $A6)</f>
+        <v>9.8476537179000037</v>
       </c>
       <c r="S6">
         <f t="shared" si="6"/>
-        <v>8.1459517916319975</v>
+        <v>10.941837464333338</v>
       </c>
       <c r="T6">
         <f t="shared" si="6"/>
-        <v>8.9605469707951979</v>
+        <v>12.036021210766672</v>
       </c>
       <c r="U6">
         <f t="shared" si="6"/>
-        <v>9.7751421499583984</v>
+        <v>13.130204957200004</v>
       </c>
       <c r="V6">
         <f t="shared" si="6"/>
-        <v>10.589737329121597</v>
+        <v>14.224388703633338</v>
       </c>
       <c r="W6">
         <f t="shared" si="6"/>
-        <v>11.404332508284797</v>
+        <v>15.318572450066672</v>
       </c>
       <c r="X6">
         <f t="shared" si="6"/>
-        <v>12.218927687447996</v>
+        <v>16.412756196500006</v>
       </c>
       <c r="Z6">
         <f t="shared" ref="Z6:Z25" si="7">R6-B6</f>
-        <v>0.2715768478367977</v>
+        <v>0.42285464940000317</v>
       </c>
       <c r="AA6">
         <f t="shared" si="3"/>
-        <v>0.26045522958399747</v>
+        <v>0.41470728033333693</v>
       </c>
       <c r="AB6">
         <f t="shared" si="3"/>
-        <v>0.24086480316799808</v>
+        <v>0.39525406066667124</v>
       </c>
       <c r="AC6">
         <f t="shared" si="3"/>
-        <v>0.21274785978239841</v>
+        <v>0.36441794920000348</v>
       </c>
       <c r="AD6">
         <f t="shared" si="3"/>
-        <v>0.17604649466559685</v>
+        <v>0.3221216431333378</v>
       </c>
       <c r="AE6">
         <f t="shared" si="3"/>
-        <v>0.13070260710079751</v>
+        <v>0.26828757806667092</v>
       </c>
       <c r="AF6">
         <f t="shared" si="3"/>
-        <v>7.6657900415996849E-2</v>
+        <v>0.20283792800000455</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>12</v>
       </c>
       <c r="B7">
         <f t="shared" si="4"/>
-        <v>6.3077176770048</v>
+        <v>8.4207969184000007</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>7.1334344744207998</v>
+        <v>9.5231280339000008</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>7.9676200799999997</v>
+        <v>10.636765</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>8.8103322025487998</v>
+        <v>11.7617848579</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>9.6616287468288</v>
+        <v>12.8982649104</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>10.5215678135568</v>
+        <v>14.046282721900001</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>11.390207699404799</v>
+        <v>15.205916118399999</v>
       </c>
       <c r="J7">
         <f t="shared" si="5"/>
-        <v>0.7884647096256</v>
+        <v>1.0525996148000001</v>
       </c>
       <c r="K7">
         <f t="shared" si="5"/>
-        <v>0.79260383049119987</v>
+        <v>1.0581253371000001</v>
       </c>
       <c r="L7">
         <f t="shared" si="5"/>
-        <v>0.79676200799999997</v>
+        <v>1.0636764999999999</v>
       </c>
       <c r="M7">
         <f t="shared" si="5"/>
-        <v>0.80093929114079987</v>
+        <v>1.0692531689</v>
       </c>
       <c r="N7">
         <f t="shared" si="5"/>
-        <v>0.80513572890239993</v>
+        <v>1.0748554092</v>
       </c>
       <c r="O7">
         <f t="shared" si="5"/>
-        <v>0.80935137027359993</v>
+        <v>1.0804832863</v>
       </c>
       <c r="P7">
         <f t="shared" si="5"/>
-        <v>0.81358626424319991</v>
+        <v>1.0861368655999999</v>
       </c>
       <c r="R7">
         <f t="shared" si="6"/>
-        <v>6.5167614333055983</v>
+        <v>8.7534699714666697</v>
       </c>
       <c r="S7">
         <f t="shared" si="6"/>
-        <v>7.3313566124687979</v>
+        <v>9.8476537179000037</v>
       </c>
       <c r="T7">
         <f t="shared" si="6"/>
-        <v>8.1459517916319975</v>
+        <v>10.941837464333338</v>
       </c>
       <c r="U7">
         <f t="shared" si="6"/>
-        <v>8.9605469707951979</v>
+        <v>12.036021210766672</v>
       </c>
       <c r="V7">
         <f t="shared" si="6"/>
-        <v>9.7751421499583984</v>
+        <v>13.130204957200004</v>
       </c>
       <c r="W7">
         <f t="shared" si="6"/>
-        <v>10.589737329121597</v>
+        <v>14.224388703633338</v>
       </c>
       <c r="X7">
         <f t="shared" si="6"/>
-        <v>11.404332508284797</v>
+        <v>15.318572450066672</v>
       </c>
       <c r="Z7">
         <f t="shared" si="7"/>
-        <v>0.2090437563007983</v>
+        <v>0.33267305306666906</v>
       </c>
       <c r="AA7">
         <f t="shared" si="3"/>
-        <v>0.19792213804799808</v>
+        <v>0.32452568400000281</v>
       </c>
       <c r="AB7">
         <f t="shared" si="3"/>
-        <v>0.17833171163199779</v>
+        <v>0.30507246433333712</v>
       </c>
       <c r="AC7">
         <f t="shared" si="3"/>
-        <v>0.15021476824639812</v>
+        <v>0.27423635286667114</v>
       </c>
       <c r="AD7">
         <f t="shared" si="3"/>
-        <v>0.11351340312959834</v>
+        <v>0.23194004680000369</v>
       </c>
       <c r="AE7">
         <f t="shared" si="3"/>
-        <v>6.8169515564797223E-2</v>
+        <v>0.1781059817333368</v>
       </c>
       <c r="AF7">
         <f t="shared" si="3"/>
-        <v>1.4124808879998341E-2</v>
+        <v>0.11265633166667222</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>13</v>
       </c>
       <c r="B8">
         <f t="shared" si="4"/>
-        <v>5.5476973424880001</v>
+        <v>7.4061705164999996</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>6.3734141399039999</v>
+        <v>8.5085016319999998</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>7.2075997454831997</v>
+        <v>9.6221385980999994</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>8.0503118680319989</v>
+        <v>10.747158455999999</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>8.9016084123119992</v>
+        <v>11.883638508500001</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>9.761547479039999</v>
+        <v>13.03165632</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>10.630187364888</v>
+        <v>14.1912897165</v>
       </c>
       <c r="J8">
         <f t="shared" si="5"/>
-        <v>0.79252819178399991</v>
+        <v>1.0580243595000001</v>
       </c>
       <c r="K8">
         <f t="shared" si="5"/>
-        <v>0.79667676748799998</v>
+        <v>1.063562704</v>
       </c>
       <c r="L8">
         <f t="shared" si="5"/>
-        <v>0.80084441616479995</v>
+        <v>1.0691265109000001</v>
       </c>
       <c r="M8">
         <f t="shared" si="5"/>
-        <v>0.80503118680320007</v>
+        <v>1.0747158456000001</v>
       </c>
       <c r="N8">
         <f t="shared" si="5"/>
-        <v>0.8092371283919999</v>
+        <v>1.0803307735000001</v>
       </c>
       <c r="O8">
         <f t="shared" si="5"/>
-        <v>0.81346228992000003</v>
+        <v>1.0859713600000001</v>
       </c>
       <c r="P8">
         <f t="shared" si="5"/>
-        <v>0.8177067203759999</v>
+        <v>1.0916376704999999</v>
       </c>
       <c r="R8">
         <f t="shared" si="6"/>
-        <v>5.7021662541423987</v>
+        <v>7.6592862250333358</v>
       </c>
       <c r="S8">
         <f t="shared" si="6"/>
-        <v>6.5167614333055983</v>
+        <v>8.7534699714666697</v>
       </c>
       <c r="T8">
         <f t="shared" si="6"/>
-        <v>7.3313566124687979</v>
+        <v>9.8476537179000037</v>
       </c>
       <c r="U8">
         <f t="shared" si="6"/>
-        <v>8.1459517916319975</v>
+        <v>10.941837464333338</v>
       </c>
       <c r="V8">
         <f t="shared" si="6"/>
-        <v>8.9605469707951979</v>
+        <v>12.036021210766672</v>
       </c>
       <c r="W8">
         <f t="shared" si="6"/>
-        <v>9.7751421499583984</v>
+        <v>13.130204957200004</v>
       </c>
       <c r="X8">
         <f t="shared" si="6"/>
-        <v>10.589737329121597</v>
+        <v>14.224388703633338</v>
       </c>
       <c r="Z8">
         <f t="shared" si="7"/>
-        <v>0.15446891165439869</v>
+        <v>0.2531157085333362</v>
       </c>
       <c r="AA8">
         <f t="shared" si="3"/>
-        <v>0.14334729340159846</v>
+        <v>0.24496833946666996</v>
       </c>
       <c r="AB8">
         <f t="shared" si="3"/>
-        <v>0.12375686698559818</v>
+        <v>0.22551511980000427</v>
       </c>
       <c r="AC8">
         <f t="shared" si="3"/>
-        <v>9.5639923599998511E-2</v>
+        <v>0.19467900833333829</v>
       </c>
       <c r="AD8">
         <f t="shared" si="3"/>
-        <v>5.8938558483198733E-2</v>
+        <v>0.15238270226667083</v>
       </c>
       <c r="AE8">
         <f t="shared" si="3"/>
-        <v>1.3594670918399387E-2</v>
+        <v>9.8548637200003952E-2</v>
       </c>
       <c r="AF8">
         <f t="shared" si="3"/>
-        <v>-4.0450035766403047E-2</v>
+        <v>3.3098987133337587E-2</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>14</v>
       </c>
       <c r="B9">
         <f t="shared" si="4"/>
-        <v>4.7796628158720003</v>
+        <v>6.3808451760000002</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>5.6053796132880001</v>
+        <v>7.4831762915000004</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>6.4395652188671999</v>
+        <v>8.5968132575999991</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>7.282277341416</v>
+        <v>9.7218331155000008</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>8.1335738856960003</v>
+        <v>10.858313168</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>8.9935129524240001</v>
+        <v>12.0063309795</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>9.8621528382719994</v>
+        <v>13.165964376</v>
       </c>
       <c r="J9">
         <f t="shared" si="5"/>
-        <v>0.79661046931199997</v>
+        <v>1.063474196</v>
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>0.80076851618399991</v>
+        <v>1.0690251845000001</v>
       </c>
       <c r="L9">
         <f t="shared" si="5"/>
-        <v>0.80494565235839999</v>
+        <v>1.0746016572000001</v>
       </c>
       <c r="M9">
         <f t="shared" si="5"/>
-        <v>0.80914192682399999</v>
+        <v>1.0802036795000001</v>
       </c>
       <c r="N9">
         <f t="shared" si="5"/>
-        <v>0.81335738856959994</v>
+        <v>1.0858313168</v>
       </c>
       <c r="O9">
         <f t="shared" si="5"/>
-        <v>0.81759208658399996</v>
+        <v>1.0914846345</v>
       </c>
       <c r="P9">
         <f t="shared" si="5"/>
-        <v>0.82184606985599995</v>
+        <v>1.0971636979999999</v>
       </c>
       <c r="R9">
         <f t="shared" si="6"/>
-        <v>4.8875710749791992</v>
+        <v>6.5651024786000018</v>
       </c>
       <c r="S9">
         <f t="shared" si="6"/>
-        <v>5.7021662541423987</v>
+        <v>7.6592862250333358</v>
       </c>
       <c r="T9">
         <f t="shared" si="6"/>
-        <v>6.5167614333055983</v>
+        <v>8.7534699714666697</v>
       </c>
       <c r="U9">
         <f t="shared" si="6"/>
-        <v>7.3313566124687979</v>
+        <v>9.8476537179000037</v>
       </c>
       <c r="V9">
         <f t="shared" si="6"/>
-        <v>8.1459517916319975</v>
+        <v>10.941837464333338</v>
       </c>
       <c r="W9">
         <f t="shared" si="6"/>
-        <v>8.9605469707951979</v>
+        <v>12.036021210766672</v>
       </c>
       <c r="X9">
         <f t="shared" si="6"/>
-        <v>9.7751421499583984</v>
+        <v>13.130204957200004</v>
       </c>
       <c r="Z9">
         <f t="shared" si="7"/>
-        <v>0.10790825910719892</v>
+        <v>0.18425730260000162</v>
       </c>
       <c r="AA9">
         <f t="shared" si="3"/>
-        <v>9.6786640854398698E-2</v>
+        <v>0.17610993353333537</v>
       </c>
       <c r="AB9">
         <f t="shared" si="3"/>
-        <v>7.7196214438398414E-2</v>
+        <v>0.15665671386667057</v>
       </c>
       <c r="AC9">
         <f t="shared" si="3"/>
-        <v>4.9079271052797857E-2</v>
+        <v>0.12582060240000281</v>
       </c>
       <c r="AD9">
         <f t="shared" si="3"/>
-        <v>1.2377905935997191E-2</v>
+        <v>8.3524296333337134E-2</v>
       </c>
       <c r="AE9">
         <f t="shared" si="3"/>
-        <v>-3.2965981628802155E-2</v>
+        <v>2.9690231266672029E-2</v>
       </c>
       <c r="AF9">
         <f t="shared" si="3"/>
-        <v>-8.7010688313601037E-2</v>
+        <v>-3.5759418799996112E-2</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>15</v>
       </c>
       <c r="B10">
         <f t="shared" si="4"/>
-        <v>4.003557955992</v>
+        <v>5.3447459485</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>4.8292747534079998</v>
+        <v>6.4470770640000001</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>5.6634603589871997</v>
+        <v>7.5607140300999998</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>6.5061724815359998</v>
+        <v>8.6857338879999997</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>7.357469025816</v>
+        <v>9.8222139404999993</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>8.2174080925439998</v>
+        <v>10.970231752</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>9.0860479783919992</v>
+        <v>12.1298651485</v>
       </c>
       <c r="J10">
         <f t="shared" si="5"/>
-        <v>0.80071159119839996</v>
+        <v>1.0689491897000001</v>
       </c>
       <c r="K10">
         <f t="shared" si="5"/>
-        <v>0.8048791255679999</v>
+        <v>1.074512844</v>
       </c>
       <c r="L10">
         <f t="shared" si="5"/>
-        <v>0.80906576556959997</v>
+        <v>1.0801020043</v>
       </c>
       <c r="M10">
         <f t="shared" si="5"/>
-        <v>0.81327156019199998</v>
+        <v>1.085716736</v>
       </c>
       <c r="N10">
         <f t="shared" si="5"/>
-        <v>0.81749655842399993</v>
+        <v>1.0913571045000001</v>
       </c>
       <c r="O10">
         <f t="shared" si="5"/>
-        <v>0.82174080925439996</v>
+        <v>1.0970231751999999</v>
       </c>
       <c r="P10">
         <f t="shared" si="5"/>
-        <v>0.82600436167199998</v>
+        <v>1.1027150134999999</v>
       </c>
       <c r="R10">
         <f t="shared" si="6"/>
-        <v>4.0729758958159987</v>
+        <v>5.4709187321666688</v>
       </c>
       <c r="S10">
         <f t="shared" si="6"/>
-        <v>4.8875710749791992</v>
+        <v>6.5651024786000018</v>
       </c>
       <c r="T10">
         <f t="shared" si="6"/>
-        <v>5.7021662541423987</v>
+        <v>7.6592862250333358</v>
       </c>
       <c r="U10">
         <f t="shared" si="6"/>
-        <v>6.5167614333055983</v>
+        <v>8.7534699714666697</v>
       </c>
       <c r="V10">
         <f t="shared" si="6"/>
-        <v>7.3313566124687979</v>
+        <v>9.8476537179000037</v>
       </c>
       <c r="W10">
         <f t="shared" si="6"/>
-        <v>8.1459517916319975</v>
+        <v>10.941837464333338</v>
       </c>
       <c r="X10">
         <f t="shared" si="6"/>
-        <v>8.9605469707951979</v>
+        <v>12.036021210766672</v>
       </c>
       <c r="Z10">
         <f t="shared" si="7"/>
-        <v>6.9417939823998687E-2</v>
+        <v>0.12617278366666884</v>
       </c>
       <c r="AA10">
         <f t="shared" si="3"/>
-        <v>5.829632157119935E-2</v>
+        <v>0.11802541460000171</v>
       </c>
       <c r="AB10">
         <f t="shared" si="3"/>
-        <v>3.8705895155199066E-2</v>
+        <v>9.8572194933336021E-2</v>
       </c>
       <c r="AC10">
         <f t="shared" si="3"/>
-        <v>1.0588951769598509E-2</v>
+        <v>6.7736083466670038E-2</v>
       </c>
       <c r="AD10">
         <f t="shared" si="3"/>
-        <v>-2.6112413347202157E-2</v>
+        <v>2.543977740000436E-2</v>
       </c>
       <c r="AE10">
         <f t="shared" si="3"/>
-        <v>-7.1456300912002391E-2</v>
+        <v>-2.8394287666662521E-2</v>
       </c>
       <c r="AF10">
         <f t="shared" si="3"/>
-        <v>-0.12550100759680127</v>
+        <v>-9.3843937733328886E-2</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>16</v>
       </c>
       <c r="B11">
         <f t="shared" si="4"/>
-        <v>3.2193264257280001</v>
+        <v>4.2977976240000002</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>4.0450432231439999</v>
+        <v>5.4001287395000004</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>4.8792288287231997</v>
+        <v>6.5137657056</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>5.7219409512719999</v>
+        <v>7.6387855634999999</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>6.5732374955520001</v>
+        <v>8.7752656160000004</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>7.4331765622799999</v>
+        <v>9.9232834274999995</v>
       </c>
       <c r="H11">
         <f t="shared" si="0"/>
-        <v>8.3018164481279992</v>
+        <v>11.082916824</v>
       </c>
       <c r="J11">
         <f t="shared" si="5"/>
-        <v>0.80483160643200002</v>
+        <v>1.0744494060000001</v>
       </c>
       <c r="K11">
         <f t="shared" si="5"/>
-        <v>0.80900864462879996</v>
+        <v>1.0800257478999999</v>
       </c>
       <c r="L11">
         <f t="shared" si="5"/>
-        <v>0.81320480478720003</v>
+        <v>1.0856276176000001</v>
       </c>
       <c r="M11">
         <f t="shared" si="5"/>
-        <v>0.81742013589599993</v>
+        <v>1.0912550805000001</v>
       </c>
       <c r="N11">
         <f t="shared" si="5"/>
-        <v>0.82165468694400001</v>
+        <v>1.0969082020000001</v>
       </c>
       <c r="O11">
         <f t="shared" si="5"/>
-        <v>0.82590850691999995</v>
+        <v>1.1025870474999999</v>
       </c>
       <c r="P11">
         <f t="shared" si="5"/>
-        <v>0.83018164481279999</v>
+        <v>1.1082916824</v>
       </c>
       <c r="R11">
         <f t="shared" si="6"/>
-        <v>3.2583807166527992</v>
+        <v>4.3767349857333349</v>
       </c>
       <c r="S11">
         <f t="shared" si="6"/>
-        <v>4.0729758958159987</v>
+        <v>5.4709187321666688</v>
       </c>
       <c r="T11">
         <f t="shared" si="6"/>
-        <v>4.8875710749791992</v>
+        <v>6.5651024786000018</v>
       </c>
       <c r="U11">
         <f t="shared" si="6"/>
-        <v>5.7021662541423987</v>
+        <v>7.6592862250333358</v>
       </c>
       <c r="V11">
         <f t="shared" si="6"/>
-        <v>6.5167614333055983</v>
+        <v>8.7534699714666697</v>
       </c>
       <c r="W11">
         <f t="shared" si="6"/>
-        <v>7.3313566124687979</v>
+        <v>9.8476537179000037</v>
       </c>
       <c r="X11">
         <f t="shared" si="6"/>
-        <v>8.1459517916319975</v>
+        <v>10.941837464333338</v>
       </c>
       <c r="Z11">
         <f t="shared" si="7"/>
-        <v>3.9054290924799062E-2</v>
+        <v>7.8937361733334654E-2</v>
       </c>
       <c r="AA11">
         <f t="shared" si="3"/>
-        <v>2.7932672671998837E-2</v>
+        <v>7.0789992666668411E-2</v>
       </c>
       <c r="AB11">
         <f t="shared" si="3"/>
-        <v>8.3422462559994415E-3</v>
+        <v>5.1336773000001834E-2</v>
       </c>
       <c r="AC11">
         <f t="shared" si="3"/>
-        <v>-1.9774697129601115E-2</v>
+        <v>2.0500661533335851E-2</v>
       </c>
       <c r="AD11">
         <f t="shared" si="3"/>
-        <v>-5.6476062246401781E-2</v>
+        <v>-2.1795644533330716E-2</v>
       </c>
       <c r="AE11">
         <f t="shared" si="3"/>
-        <v>-0.10181994981120202</v>
+        <v>-7.562970959999582E-2</v>
       </c>
       <c r="AF11">
         <f t="shared" si="3"/>
-        <v>-0.15586465649600179</v>
+        <v>-0.14107935966666219</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>17</v>
       </c>
       <c r="B12">
         <f t="shared" si="4"/>
-        <v>2.4269116920047997</v>
+        <v>3.2399247308999999</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>3.2526284894208</v>
+        <v>4.3422558463999996</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>4.0868140950000003</v>
+        <v>5.4558928125000001</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>4.9295262175487995</v>
+        <v>6.5809126704000001</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>5.7808227618287997</v>
+        <v>7.7173927228999997</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>6.6407618285567995</v>
+        <v>8.8654105344000005</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>7.5094017144047998</v>
+        <v>10.025043930900001</v>
       </c>
       <c r="J12">
         <f t="shared" si="5"/>
-        <v>0.80897056400159995</v>
+        <v>1.0799749103</v>
       </c>
       <c r="K12">
         <f t="shared" si="5"/>
-        <v>0.81315712235519999</v>
+        <v>1.0855639615999999</v>
       </c>
       <c r="L12">
         <f t="shared" si="5"/>
-        <v>0.81736281899999996</v>
+        <v>1.0911785625000001</v>
       </c>
       <c r="M12">
         <f t="shared" si="5"/>
-        <v>0.82158770292479999</v>
+        <v>1.0968187784000001</v>
       </c>
       <c r="N12">
         <f t="shared" si="5"/>
-        <v>0.82583182311839998</v>
+        <v>1.1024846746999999</v>
       </c>
       <c r="O12">
         <f t="shared" si="5"/>
-        <v>0.83009522856959994</v>
+        <v>1.1081763168000001</v>
       </c>
       <c r="P12">
         <f t="shared" si="5"/>
-        <v>0.83437796826720001</v>
+        <v>1.1138937701</v>
       </c>
       <c r="R12">
         <f t="shared" si="6"/>
-        <v>2.4437855374895996</v>
+        <v>3.2825512393000009</v>
       </c>
       <c r="S12">
         <f t="shared" si="6"/>
-        <v>3.2583807166527992</v>
+        <v>4.3767349857333349</v>
       </c>
       <c r="T12">
         <f t="shared" si="6"/>
-        <v>4.0729758958159987</v>
+        <v>5.4709187321666688</v>
       </c>
       <c r="U12">
         <f t="shared" si="6"/>
-        <v>4.8875710749791992</v>
+        <v>6.5651024786000018</v>
       </c>
       <c r="V12">
         <f t="shared" si="6"/>
-        <v>5.7021662541423987</v>
+        <v>7.6592862250333358</v>
       </c>
       <c r="W12">
         <f t="shared" si="6"/>
-        <v>6.5167614333055983</v>
+        <v>8.7534699714666697</v>
       </c>
       <c r="X12">
         <f t="shared" si="6"/>
-        <v>7.3313566124687979</v>
+        <v>9.8476537179000037</v>
       </c>
       <c r="Z12">
         <f t="shared" si="7"/>
-        <v>1.6873845484799865E-2</v>
+        <v>4.262650840000104E-2</v>
       </c>
       <c r="AA12">
         <f t="shared" si="3"/>
-        <v>5.7522272319991963E-3</v>
+        <v>3.447913933333524E-2</v>
       </c>
       <c r="AB12">
         <f t="shared" si="3"/>
-        <v>-1.3838199184001532E-2</v>
+        <v>1.5025919666668663E-2</v>
       </c>
       <c r="AC12">
         <f t="shared" si="3"/>
-        <v>-4.1955142569600312E-2</v>
+        <v>-1.5810191799998208E-2</v>
       </c>
       <c r="AD12">
         <f t="shared" si="3"/>
-        <v>-7.8656507686400978E-2</v>
+        <v>-5.8106497866663886E-2</v>
       </c>
       <c r="AE12">
         <f t="shared" si="3"/>
-        <v>-0.12400039525120121</v>
+        <v>-0.11194056293333077</v>
       </c>
       <c r="AF12">
         <f t="shared" si="3"/>
-        <v>-0.17804510193600187</v>
+        <v>-0.17739021299999713</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>18</v>
       </c>
       <c r="B13">
         <f t="shared" si="4"/>
-        <v>1.6262570257919999</v>
+        <v>2.1710515359999998</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>2.4519738232079997</v>
+        <v>3.2733826515</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>3.2861594287872</v>
+        <v>4.3870196176</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>4.1288715513360001</v>
+        <v>5.5120394755</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>4.9801680956159995</v>
+        <v>6.6485195279999996</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>5.8401071623440002</v>
+        <v>7.7965373395000004</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>6.7087470481919995</v>
+        <v>8.9561707360000007</v>
       </c>
       <c r="J13">
         <f t="shared" si="5"/>
-        <v>0.81312851289599997</v>
+        <v>1.0855257680000001</v>
       </c>
       <c r="K13">
         <f t="shared" si="5"/>
-        <v>0.81732460773600002</v>
+        <v>1.0911275505</v>
       </c>
       <c r="L13">
         <f t="shared" si="5"/>
-        <v>0.82153985719680001</v>
+        <v>1.0967549044</v>
       </c>
       <c r="M13">
         <f t="shared" si="5"/>
-        <v>0.82577431026719994</v>
+        <v>1.1024078951</v>
       </c>
       <c r="N13">
         <f t="shared" si="5"/>
-        <v>0.83002801593600006</v>
+        <v>1.1080865879999999</v>
       </c>
       <c r="O13">
         <f t="shared" si="5"/>
-        <v>0.83430102319199995</v>
+        <v>1.1137910485</v>
       </c>
       <c r="P13">
         <f t="shared" si="5"/>
-        <v>0.83859338102400005</v>
+        <v>1.1195213419999999</v>
       </c>
       <c r="R13">
         <f t="shared" si="6"/>
-        <v>1.6291903583263996</v>
+        <v>2.1883674928666674</v>
       </c>
       <c r="S13">
         <f t="shared" si="6"/>
-        <v>2.4437855374895996</v>
+        <v>3.2825512393000009</v>
       </c>
       <c r="T13">
         <f t="shared" si="6"/>
-        <v>3.2583807166527992</v>
+        <v>4.3767349857333349</v>
       </c>
       <c r="U13">
         <f t="shared" si="6"/>
-        <v>4.0729758958159987</v>
+        <v>5.4709187321666688</v>
       </c>
       <c r="V13">
         <f t="shared" si="6"/>
-        <v>4.8875710749791992</v>
+        <v>6.5651024786000018</v>
       </c>
       <c r="W13">
         <f t="shared" si="6"/>
-        <v>5.7021662541423987</v>
+        <v>7.6592862250333358</v>
       </c>
       <c r="X13">
         <f t="shared" si="6"/>
-        <v>6.5167614333055983</v>
+        <v>8.7534699714666697</v>
       </c>
       <c r="Z13">
         <f t="shared" si="7"/>
-        <v>2.9333325343996464E-3</v>
+        <v>1.7315956866667648E-2</v>
       </c>
       <c r="AA13">
         <f t="shared" si="3"/>
-        <v>-8.1882857184001345E-3</v>
+        <v>9.1685878000009602E-3</v>
       </c>
       <c r="AB13">
         <f t="shared" si="3"/>
-        <v>-2.7778712134400863E-2</v>
+        <v>-1.0284631866665173E-2</v>
       </c>
       <c r="AC13">
         <f t="shared" si="3"/>
-        <v>-5.5895655520001419E-2</v>
+        <v>-4.1120743333331156E-2</v>
       </c>
       <c r="AD13">
         <f t="shared" si="3"/>
-        <v>-9.2597020636800309E-2</v>
+        <v>-8.3417049399997723E-2</v>
       </c>
       <c r="AE13">
         <f t="shared" si="3"/>
-        <v>-0.13794090820160143</v>
+        <v>-0.1372511144666646</v>
       </c>
       <c r="AF13">
         <f t="shared" si="3"/>
-        <v>-0.1919856148864012</v>
+        <v>-0.20270076453333097</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>19</v>
       </c>
       <c r="B14">
         <f t="shared" si="4"/>
-        <v>0.81730550210399999</v>
+        <v>1.0911020444999999</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>1.6430222995199999</v>
+        <v>2.1934331600000001</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>2.4772079050992</v>
+        <v>3.3070701261000002</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>3.3199200276480001</v>
+        <v>4.4320899840000001</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>4.1712165719279994</v>
+        <v>5.5685700364999997</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
-        <v>5.0311556386560001</v>
+        <v>6.7165878479999996</v>
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>5.8997955245039995</v>
+        <v>7.8762212444999999</v>
       </c>
       <c r="J14">
         <f t="shared" si="5"/>
-        <v>0.81730550210399999</v>
+        <v>1.0911020444999999</v>
       </c>
       <c r="K14">
         <f t="shared" si="5"/>
-        <v>0.82151114975999995</v>
+        <v>1.0967165800000001</v>
       </c>
       <c r="L14">
         <f t="shared" si="5"/>
-        <v>0.82573596836639995</v>
+        <v>1.1023567086999999</v>
       </c>
       <c r="M14">
         <f t="shared" si="5"/>
-        <v>0.82998000691199991</v>
+        <v>1.108022496</v>
       </c>
       <c r="N14">
         <f t="shared" si="5"/>
-        <v>0.83424331438559995</v>
+        <v>1.1137140073</v>
       </c>
       <c r="O14">
         <f t="shared" si="5"/>
-        <v>0.83852593977599998</v>
+        <v>1.119431308</v>
       </c>
       <c r="P14">
         <f t="shared" si="5"/>
-        <v>0.84282793207200002</v>
+        <v>1.1251744635000001</v>
       </c>
       <c r="R14">
         <f t="shared" si="6"/>
-        <v>0.81459517916319979</v>
+        <v>1.0941837464333337</v>
       </c>
       <c r="S14">
         <f t="shared" si="6"/>
-        <v>1.6291903583263996</v>
+        <v>2.1883674928666674</v>
       </c>
       <c r="T14">
         <f t="shared" si="6"/>
-        <v>2.4437855374895996</v>
+        <v>3.2825512393000009</v>
       </c>
       <c r="U14">
         <f t="shared" si="6"/>
-        <v>3.2583807166527992</v>
+        <v>4.3767349857333349</v>
       </c>
       <c r="V14">
         <f t="shared" si="6"/>
-        <v>4.0729758958159987</v>
+        <v>5.4709187321666688</v>
       </c>
       <c r="W14">
         <f t="shared" si="6"/>
-        <v>4.8875710749791992</v>
+        <v>6.5651024786000018</v>
       </c>
       <c r="X14">
         <f t="shared" si="6"/>
-        <v>5.7021662541423987</v>
+        <v>7.6592862250333358</v>
       </c>
       <c r="Z14">
         <f t="shared" si="7"/>
-        <v>-2.7103229408002028E-3</v>
+        <v>3.0817019333337914E-3</v>
       </c>
       <c r="AA14">
         <f t="shared" si="3"/>
-        <v>-1.3831941193600317E-2</v>
+        <v>-5.0656671333326742E-3</v>
       </c>
       <c r="AB14">
         <f t="shared" si="3"/>
-        <v>-3.3422367609600379E-2</v>
+        <v>-2.4518886799999251E-2</v>
       </c>
       <c r="AC14">
         <f t="shared" si="3"/>
-        <v>-6.1539310995200935E-2</v>
+        <v>-5.5354998266665234E-2</v>
       </c>
       <c r="AD14">
         <f t="shared" si="3"/>
-        <v>-9.8240676112000713E-2</v>
+        <v>-9.7651304333330913E-2</v>
       </c>
       <c r="AE14">
         <f t="shared" si="3"/>
-        <v>-0.14358456367680095</v>
+        <v>-0.15148536939999779</v>
       </c>
       <c r="AF14">
         <f t="shared" si="3"/>
-        <v>-0.19762927036160072</v>
+        <v>-0.21693501946666416</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>20</v>
       </c>
       <c r="B15">
@@ -3421,55 +3466,55 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>0.82571679741600001</v>
+        <v>1.1023311155</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>1.6599024029951999</v>
+        <v>2.2159680815999998</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>2.5026145255439998</v>
+        <v>3.3409879395000002</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>3.353911069824</v>
+        <v>4.4774679920000002</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>4.2138501365519998</v>
+        <v>5.6254858035000002</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>5.0824900224</v>
+        <v>6.7851191999999996</v>
       </c>
       <c r="J15">
         <f t="shared" si="5"/>
-        <v>0.82150158061440004</v>
+        <v>1.0967038052</v>
       </c>
       <c r="K15">
         <f t="shared" si="5"/>
-        <v>0.82571679741600001</v>
+        <v>1.1023311155</v>
       </c>
       <c r="L15">
         <f t="shared" si="5"/>
-        <v>0.82995120149760004</v>
+        <v>1.1079840407999999</v>
       </c>
       <c r="M15">
         <f t="shared" si="5"/>
-        <v>0.83420484184800003</v>
+        <v>1.1136626465000001</v>
       </c>
       <c r="N15">
         <f t="shared" si="5"/>
-        <v>0.838477767456</v>
+        <v>1.1193669980000001</v>
       </c>
       <c r="O15">
         <f t="shared" si="5"/>
-        <v>0.84277002731039996</v>
+        <v>1.1250971607</v>
       </c>
       <c r="P15">
         <f t="shared" si="5"/>
-        <v>0.84708167040000004</v>
+        <v>1.1308532</v>
       </c>
       <c r="R15">
         <f t="shared" si="6"/>
@@ -3477,27 +3522,27 @@
       </c>
       <c r="S15">
         <f t="shared" si="6"/>
-        <v>0.81459517916319979</v>
+        <v>1.0941837464333337</v>
       </c>
       <c r="T15">
         <f t="shared" si="6"/>
-        <v>1.6291903583263996</v>
+        <v>2.1883674928666674</v>
       </c>
       <c r="U15">
         <f t="shared" si="6"/>
-        <v>2.4437855374895996</v>
+        <v>3.2825512393000009</v>
       </c>
       <c r="V15">
         <f t="shared" si="6"/>
-        <v>3.2583807166527992</v>
+        <v>4.3767349857333349</v>
       </c>
       <c r="W15">
         <f t="shared" si="6"/>
-        <v>4.0729758958159987</v>
+        <v>5.4709187321666688</v>
       </c>
       <c r="X15">
         <f t="shared" si="6"/>
-        <v>4.8875710749791992</v>
+        <v>6.5651024786000018</v>
       </c>
       <c r="Z15">
         <f t="shared" si="7"/>
@@ -3505,36 +3550,36 @@
       </c>
       <c r="AA15">
         <f t="shared" si="3"/>
-        <v>-1.1121618252800225E-2</v>
+        <v>-8.1473690666662435E-3</v>
       </c>
       <c r="AB15">
         <f t="shared" si="3"/>
-        <v>-3.0712044668800287E-2</v>
+        <v>-2.7600588733332376E-2</v>
       </c>
       <c r="AC15">
         <f t="shared" si="3"/>
-        <v>-5.8828988054400178E-2</v>
+        <v>-5.8436700199999247E-2</v>
       </c>
       <c r="AD15">
         <f t="shared" si="3"/>
-        <v>-9.5530353171200844E-2</v>
+        <v>-0.10073300626666537</v>
       </c>
       <c r="AE15">
         <f t="shared" si="3"/>
-        <v>-0.14087424073600108</v>
+        <v>-0.15456707133333136</v>
       </c>
       <c r="AF15">
         <f t="shared" si="3"/>
-        <v>-0.19491894742080085</v>
+        <v>-0.22001672139999773</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>21</v>
       </c>
       <c r="B16">
         <f t="shared" si="4"/>
-        <v>-0.82571679741600001</v>
+        <v>-1.1023311155</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
@@ -3542,55 +3587,55 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>0.83418560557919996</v>
+        <v>1.1136369661000001</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>1.676897728128</v>
+        <v>2.238656824</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>2.5281942724079998</v>
+        <v>3.3751368765</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>3.388133339136</v>
+        <v>4.523154688</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>4.2567732249840002</v>
+        <v>5.6827880845000003</v>
       </c>
       <c r="J16">
         <f t="shared" si="5"/>
-        <v>0.82571679741600001</v>
+        <v>1.1023311155</v>
       </c>
       <c r="K16">
         <f t="shared" si="5"/>
-        <v>0.82994159969280001</v>
+        <v>1.1079712224</v>
       </c>
       <c r="L16">
         <f t="shared" si="5"/>
-        <v>0.83418560557919996</v>
+        <v>1.1136369661000001</v>
       </c>
       <c r="M16">
         <f t="shared" si="5"/>
-        <v>0.83844886406399999</v>
+        <v>1.119328412</v>
       </c>
       <c r="N16">
         <f t="shared" si="5"/>
-        <v>0.842731424136</v>
+        <v>1.1250456255000001</v>
       </c>
       <c r="O16">
         <f t="shared" si="5"/>
-        <v>0.847033334784</v>
+        <v>1.130788672</v>
       </c>
       <c r="P16">
         <f t="shared" si="5"/>
-        <v>0.85135464499680003</v>
+        <v>1.1365576169</v>
       </c>
       <c r="R16">
         <f t="shared" si="6"/>
-        <v>-0.81459517916319979</v>
+        <v>-1.0941837464333337</v>
       </c>
       <c r="S16">
         <f t="shared" si="6"/>
@@ -3598,27 +3643,27 @@
       </c>
       <c r="T16">
         <f t="shared" si="6"/>
-        <v>0.81459517916319979</v>
+        <v>1.0941837464333337</v>
       </c>
       <c r="U16">
         <f t="shared" si="6"/>
-        <v>1.6291903583263996</v>
+        <v>2.1883674928666674</v>
       </c>
       <c r="V16">
         <f t="shared" si="6"/>
-        <v>2.4437855374895996</v>
+        <v>3.2825512393000009</v>
       </c>
       <c r="W16">
         <f t="shared" si="6"/>
-        <v>3.2583807166527992</v>
+        <v>4.3767349857333349</v>
       </c>
       <c r="X16">
         <f t="shared" si="6"/>
-        <v>4.0729758958159987</v>
+        <v>5.4709187321666688</v>
       </c>
       <c r="Z16">
         <f t="shared" si="7"/>
-        <v>1.1121618252800225E-2</v>
+        <v>8.1473690666662435E-3</v>
       </c>
       <c r="AA16">
         <f t="shared" si="3"/>
@@ -3626,36 +3671,36 @@
       </c>
       <c r="AB16">
         <f t="shared" si="3"/>
-        <v>-1.9590426416000173E-2</v>
+        <v>-1.9453219666666355E-2</v>
       </c>
       <c r="AC16">
         <f t="shared" si="3"/>
-        <v>-4.7707369801600397E-2</v>
+        <v>-5.028933113333256E-2</v>
       </c>
       <c r="AD16">
         <f t="shared" si="3"/>
-        <v>-8.4408734918400175E-2</v>
+        <v>-9.2585637199999127E-2</v>
       </c>
       <c r="AE16">
         <f t="shared" si="3"/>
-        <v>-0.12975262248320085</v>
+        <v>-0.14641970226666512</v>
       </c>
       <c r="AF16">
         <f t="shared" si="3"/>
-        <v>-0.18379732916800151</v>
+        <v>-0.21186935233333148</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>22</v>
       </c>
       <c r="B17">
         <f t="shared" si="4"/>
-        <v>-1.6599024029951999</v>
+        <v>-2.2159680815999998</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>-0.83418560557919996</v>
+        <v>-1.1136369661000001</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
@@ -3663,55 +3708,55 @@
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>0.84271212254880001</v>
+        <v>1.1250198578999999</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>1.6940086668287999</v>
+        <v>2.2614999104</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>2.5539477335567997</v>
+        <v>3.4095177218999999</v>
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>3.4225876194047999</v>
+        <v>4.5691511183999998</v>
       </c>
       <c r="J17">
         <f t="shared" si="5"/>
-        <v>0.82995120149760004</v>
+        <v>1.1079840407999999</v>
       </c>
       <c r="K17">
         <f t="shared" si="5"/>
-        <v>0.83418560557919996</v>
+        <v>1.1136369661000001</v>
       </c>
       <c r="L17">
         <f t="shared" si="5"/>
-        <v>0.83843922960000006</v>
+        <v>1.11931555</v>
       </c>
       <c r="M17">
         <f t="shared" si="5"/>
-        <v>0.84271212254880001</v>
+        <v>1.1250198578999999</v>
       </c>
       <c r="N17">
         <f t="shared" si="5"/>
-        <v>0.84700433341440007</v>
+        <v>1.1307499552</v>
       </c>
       <c r="O17">
         <f t="shared" si="5"/>
-        <v>0.85131591118560002</v>
+        <v>1.1365059072999999</v>
       </c>
       <c r="P17">
         <f t="shared" si="5"/>
-        <v>0.85564690485119999</v>
+        <v>1.1422877795999999</v>
       </c>
       <c r="R17">
         <f t="shared" si="6"/>
-        <v>-1.6291903583263996</v>
+        <v>-2.1883674928666674</v>
       </c>
       <c r="S17">
         <f t="shared" si="6"/>
-        <v>-0.81459517916319979</v>
+        <v>-1.0941837464333337</v>
       </c>
       <c r="T17">
         <f t="shared" si="6"/>
@@ -3719,27 +3764,27 @@
       </c>
       <c r="U17">
         <f t="shared" si="6"/>
-        <v>0.81459517916319979</v>
+        <v>1.0941837464333337</v>
       </c>
       <c r="V17">
         <f t="shared" si="6"/>
-        <v>1.6291903583263996</v>
+        <v>2.1883674928666674</v>
       </c>
       <c r="W17">
         <f t="shared" si="6"/>
-        <v>2.4437855374895996</v>
+        <v>3.2825512393000009</v>
       </c>
       <c r="X17">
         <f t="shared" si="6"/>
-        <v>3.2583807166527992</v>
+        <v>4.3767349857333349</v>
       </c>
       <c r="Z17">
         <f t="shared" si="7"/>
-        <v>3.0712044668800287E-2</v>
+        <v>2.7600588733332376E-2</v>
       </c>
       <c r="AA17">
         <f t="shared" si="3"/>
-        <v>1.9590426416000173E-2</v>
+        <v>1.9453219666666355E-2</v>
       </c>
       <c r="AB17">
         <f t="shared" si="3"/>
@@ -3747,36 +3792,36 @@
       </c>
       <c r="AC17">
         <f t="shared" si="3"/>
-        <v>-2.8116943385600224E-2</v>
+        <v>-3.0836111466666205E-2</v>
       </c>
       <c r="AD17">
         <f t="shared" si="3"/>
-        <v>-6.4818308502400335E-2</v>
+        <v>-7.313241753333255E-2</v>
       </c>
       <c r="AE17">
         <f t="shared" si="3"/>
-        <v>-0.11016219606720012</v>
+        <v>-0.12696648259999899</v>
       </c>
       <c r="AF17">
         <f t="shared" si="3"/>
-        <v>-0.16420690275200078</v>
+        <v>-0.19241613266666491</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>23</v>
       </c>
       <c r="B18">
         <f t="shared" si="4"/>
-        <v>-2.5026145255439998</v>
+        <v>-3.3409879395000002</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>-1.676897728128</v>
+        <v>-2.238656824</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>-0.84271212254880001</v>
+        <v>-1.1250198578999999</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
@@ -3784,55 +3829,55 @@
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>0.85129654428000001</v>
+        <v>1.1364800525000001</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>1.711235611008</v>
+        <v>2.284497864</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>2.5798754968559998</v>
+        <v>3.4441312604999998</v>
       </c>
       <c r="J18">
         <f t="shared" si="5"/>
-        <v>0.83420484184800003</v>
+        <v>1.1136626465000001</v>
       </c>
       <c r="K18">
         <f t="shared" si="5"/>
-        <v>0.83844886406399999</v>
+        <v>1.119328412</v>
       </c>
       <c r="L18">
         <f t="shared" si="5"/>
-        <v>0.84271212254880001</v>
+        <v>1.1250198578999999</v>
       </c>
       <c r="M18">
         <f t="shared" si="5"/>
-        <v>0.84699466629120002</v>
+        <v>1.1307370496</v>
       </c>
       <c r="N18">
         <f t="shared" si="5"/>
-        <v>0.85129654428000001</v>
+        <v>1.1364800525000001</v>
       </c>
       <c r="O18">
         <f t="shared" si="5"/>
-        <v>0.85561780550399991</v>
+        <v>1.142248932</v>
       </c>
       <c r="P18">
         <f t="shared" si="5"/>
-        <v>0.85995849895199994</v>
+        <v>1.1480437535000001</v>
       </c>
       <c r="R18">
         <f t="shared" si="6"/>
-        <v>-2.4437855374895996</v>
+        <v>-3.2825512393000009</v>
       </c>
       <c r="S18">
         <f t="shared" si="6"/>
-        <v>-1.6291903583263996</v>
+        <v>-2.1883674928666674</v>
       </c>
       <c r="T18">
         <f t="shared" si="6"/>
-        <v>-0.81459517916319979</v>
+        <v>-1.0941837464333337</v>
       </c>
       <c r="U18">
         <f t="shared" si="6"/>
@@ -3840,27 +3885,27 @@
       </c>
       <c r="V18">
         <f t="shared" si="6"/>
-        <v>0.81459517916319979</v>
+        <v>1.0941837464333337</v>
       </c>
       <c r="W18">
         <f t="shared" si="6"/>
-        <v>1.6291903583263996</v>
+        <v>2.1883674928666674</v>
       </c>
       <c r="X18">
         <f t="shared" si="6"/>
-        <v>2.4437855374895996</v>
+        <v>3.2825512393000009</v>
       </c>
       <c r="Z18">
         <f t="shared" si="7"/>
-        <v>5.8828988054400178E-2</v>
+        <v>5.8436700199999247E-2</v>
       </c>
       <c r="AA18">
         <f t="shared" si="3"/>
-        <v>4.7707369801600397E-2</v>
+        <v>5.028933113333256E-2</v>
       </c>
       <c r="AB18">
         <f t="shared" si="3"/>
-        <v>2.8116943385600224E-2</v>
+        <v>3.0836111466666205E-2</v>
       </c>
       <c r="AC18">
         <f t="shared" si="3"/>
@@ -3868,36 +3913,36 @@
       </c>
       <c r="AD18">
         <f t="shared" si="3"/>
-        <v>-3.6701365116800222E-2</v>
+        <v>-4.2296306066666345E-2</v>
       </c>
       <c r="AE18">
         <f t="shared" si="3"/>
-        <v>-8.2045252681600456E-2</v>
+        <v>-9.6130371133332559E-2</v>
       </c>
       <c r="AF18">
         <f t="shared" si="3"/>
-        <v>-0.13608995936640023</v>
+        <v>-0.16158002119999892</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>24</v>
       </c>
       <c r="B19">
         <f t="shared" si="4"/>
-        <v>-3.353911069824</v>
+        <v>-4.4774679920000002</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>-2.5281942724079998</v>
+        <v>-3.3751368765</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>-1.6940086668287999</v>
+        <v>-2.2614999104</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>-0.85129654428000001</v>
+        <v>-1.1364800525000001</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
@@ -3905,55 +3950,55 @@
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>0.85993906672800002</v>
+        <v>1.1480178114999999</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>1.728578952576</v>
+        <v>2.3076512079999998</v>
       </c>
       <c r="J19">
         <f t="shared" si="5"/>
-        <v>0.838477767456</v>
+        <v>1.1193669980000001</v>
       </c>
       <c r="K19">
         <f t="shared" si="5"/>
-        <v>0.842731424136</v>
+        <v>1.1250456255000001</v>
       </c>
       <c r="L19">
         <f t="shared" si="5"/>
-        <v>0.84700433341440007</v>
+        <v>1.1307499552</v>
       </c>
       <c r="M19">
         <f t="shared" si="5"/>
-        <v>0.85129654428000001</v>
+        <v>1.1364800525000001</v>
       </c>
       <c r="N19">
         <f t="shared" si="5"/>
-        <v>0.85560810572160007</v>
+        <v>1.1422359827999999</v>
       </c>
       <c r="O19">
         <f t="shared" si="5"/>
-        <v>0.85993906672800002</v>
+        <v>1.1480178115000002</v>
       </c>
       <c r="P19">
         <f t="shared" si="5"/>
-        <v>0.86428947628800001</v>
+        <v>1.1538256039999999</v>
       </c>
       <c r="R19">
         <f t="shared" si="6"/>
-        <v>-3.2583807166527992</v>
+        <v>-4.3767349857333349</v>
       </c>
       <c r="S19">
         <f t="shared" si="6"/>
-        <v>-2.4437855374895996</v>
+        <v>-3.2825512393000009</v>
       </c>
       <c r="T19">
         <f t="shared" si="6"/>
-        <v>-1.6291903583263996</v>
+        <v>-2.1883674928666674</v>
       </c>
       <c r="U19">
         <f t="shared" si="6"/>
-        <v>-0.81459517916319979</v>
+        <v>-1.0941837464333337</v>
       </c>
       <c r="V19">
         <f t="shared" si="6"/>
@@ -3961,27 +4006,27 @@
       </c>
       <c r="W19">
         <f t="shared" si="6"/>
-        <v>0.81459517916319979</v>
+        <v>1.0941837464333337</v>
       </c>
       <c r="X19">
         <f t="shared" si="6"/>
-        <v>1.6291903583263996</v>
+        <v>2.1883674928666674</v>
       </c>
       <c r="Z19">
         <f t="shared" si="7"/>
-        <v>9.5530353171200844E-2</v>
+        <v>0.10073300626666537</v>
       </c>
       <c r="AA19">
         <f t="shared" si="3"/>
-        <v>8.4408734918400175E-2</v>
+        <v>9.2585637199999127E-2</v>
       </c>
       <c r="AB19">
         <f t="shared" si="3"/>
-        <v>6.4818308502400335E-2</v>
+        <v>7.313241753333255E-2</v>
       </c>
       <c r="AC19">
         <f t="shared" si="3"/>
-        <v>3.6701365116800222E-2</v>
+        <v>4.2296306066666345E-2</v>
       </c>
       <c r="AD19">
         <f t="shared" si="3"/>
@@ -3989,36 +4034,36 @@
       </c>
       <c r="AE19">
         <f t="shared" si="3"/>
-        <v>-4.5343887564800234E-2</v>
+        <v>-5.3834065066666215E-2</v>
       </c>
       <c r="AF19">
         <f t="shared" si="3"/>
-        <v>-9.9388594249600448E-2</v>
+        <v>-0.11928371513333236</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>25</v>
       </c>
       <c r="B20">
         <f t="shared" si="4"/>
-        <v>-4.2138501365519998</v>
+        <v>-5.6254858035000002</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>-3.388133339136</v>
+        <v>-4.523154688</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>-2.5539477335567997</v>
+        <v>-3.4095177218999999</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>-1.711235611008</v>
+        <v>-2.284497864</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>-0.85993906672800002</v>
+        <v>-1.1480178114999999</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
@@ -4026,55 +4071,55 @@
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
-        <v>0.868639885848</v>
+        <v>1.1596333965000001</v>
       </c>
       <c r="J20">
         <f t="shared" si="5"/>
-        <v>0.84277002731039996</v>
+        <v>1.1250971607</v>
       </c>
       <c r="K20">
         <f t="shared" si="5"/>
-        <v>0.847033334784</v>
+        <v>1.130788672</v>
       </c>
       <c r="L20">
         <f t="shared" si="5"/>
-        <v>0.85131591118560002</v>
+        <v>1.1365059072999999</v>
       </c>
       <c r="M20">
         <f t="shared" si="5"/>
-        <v>0.85561780550399991</v>
+        <v>1.142248932</v>
       </c>
       <c r="N20">
         <f t="shared" si="5"/>
-        <v>0.85993906672800002</v>
+        <v>1.1480178115000002</v>
       </c>
       <c r="O20">
         <f t="shared" si="5"/>
-        <v>0.86427974384639994</v>
+        <v>1.1538126112</v>
       </c>
       <c r="P20">
         <f t="shared" si="5"/>
-        <v>0.868639885848</v>
+        <v>1.1596333965000001</v>
       </c>
       <c r="R20">
         <f t="shared" si="6"/>
-        <v>-4.0729758958159987</v>
+        <v>-5.4709187321666688</v>
       </c>
       <c r="S20">
         <f t="shared" si="6"/>
-        <v>-3.2583807166527992</v>
+        <v>-4.3767349857333349</v>
       </c>
       <c r="T20">
         <f t="shared" si="6"/>
-        <v>-2.4437855374895996</v>
+        <v>-3.2825512393000009</v>
       </c>
       <c r="U20">
         <f t="shared" si="6"/>
-        <v>-1.6291903583263996</v>
+        <v>-2.1883674928666674</v>
       </c>
       <c r="V20">
         <f t="shared" si="6"/>
-        <v>-0.81459517916319979</v>
+        <v>-1.0941837464333337</v>
       </c>
       <c r="W20">
         <f t="shared" si="6"/>
@@ -4082,27 +4127,27 @@
       </c>
       <c r="X20">
         <f t="shared" si="6"/>
-        <v>0.81459517916319979</v>
+        <v>1.0941837464333337</v>
       </c>
       <c r="Z20">
         <f t="shared" si="7"/>
-        <v>0.14087424073600108</v>
+        <v>0.15456707133333136</v>
       </c>
       <c r="AA20">
         <f t="shared" si="3"/>
-        <v>0.12975262248320085</v>
+        <v>0.14641970226666512</v>
       </c>
       <c r="AB20">
         <f t="shared" si="3"/>
-        <v>0.11016219606720012</v>
+        <v>0.12696648259999899</v>
       </c>
       <c r="AC20">
         <f t="shared" si="3"/>
-        <v>8.2045252681600456E-2</v>
+        <v>9.6130371133332559E-2</v>
       </c>
       <c r="AD20">
         <f t="shared" si="3"/>
-        <v>4.5343887564800234E-2</v>
+        <v>5.3834065066666215E-2</v>
       </c>
       <c r="AE20">
         <f t="shared" si="3"/>
@@ -4110,36 +4155,36 @@
       </c>
       <c r="AF20">
         <f t="shared" si="3"/>
-        <v>-5.4044706684800214E-2</v>
+        <v>-6.5449650066666365E-2</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>26</v>
       </c>
       <c r="B21">
         <f t="shared" si="4"/>
-        <v>-5.0824900224</v>
+        <v>-6.7851191999999996</v>
       </c>
       <c r="C21">
         <f t="shared" si="4"/>
-        <v>-4.2567732249840002</v>
+        <v>-5.6827880845000003</v>
       </c>
       <c r="D21">
         <f t="shared" si="4"/>
-        <v>-3.4225876194047999</v>
+        <v>-4.5691511183999998</v>
       </c>
       <c r="E21">
         <f t="shared" si="4"/>
-        <v>-2.5798754968559998</v>
+        <v>-3.4441312604999998</v>
       </c>
       <c r="F21">
         <f t="shared" si="4"/>
-        <v>-1.728578952576</v>
+        <v>-2.3076512079999998</v>
       </c>
       <c r="G21">
         <f t="shared" si="4"/>
-        <v>-0.868639885848</v>
+        <v>-1.1596333965000001</v>
       </c>
       <c r="H21">
         <f t="shared" si="4"/>
@@ -4147,55 +4192,55 @@
       </c>
       <c r="J21">
         <f t="shared" si="5"/>
-        <v>0.84708167040000004</v>
+        <v>1.1308532</v>
       </c>
       <c r="K21">
         <f t="shared" si="5"/>
-        <v>0.85135464499680003</v>
+        <v>1.1365576169</v>
       </c>
       <c r="L21">
         <f t="shared" si="5"/>
-        <v>0.85564690485119999</v>
+        <v>1.1422877795999999</v>
       </c>
       <c r="M21">
         <f t="shared" si="5"/>
-        <v>0.85995849895199994</v>
+        <v>1.1480437535000001</v>
       </c>
       <c r="N21">
         <f t="shared" si="5"/>
-        <v>0.86428947628800001</v>
+        <v>1.1538256039999999</v>
       </c>
       <c r="O21">
         <f t="shared" si="5"/>
-        <v>0.868639885848</v>
+        <v>1.1596333965000001</v>
       </c>
       <c r="P21">
         <f t="shared" si="5"/>
-        <v>0.87300977662080004</v>
+        <v>1.1654671964000001</v>
       </c>
       <c r="R21">
         <f t="shared" si="6"/>
-        <v>-4.8875710749791992</v>
+        <v>-6.5651024786000018</v>
       </c>
       <c r="S21">
         <f t="shared" si="6"/>
-        <v>-4.0729758958159987</v>
+        <v>-5.4709187321666688</v>
       </c>
       <c r="T21">
         <f t="shared" si="6"/>
-        <v>-3.2583807166527992</v>
+        <v>-4.3767349857333349</v>
       </c>
       <c r="U21">
         <f t="shared" si="6"/>
-        <v>-2.4437855374895996</v>
+        <v>-3.2825512393000009</v>
       </c>
       <c r="V21">
         <f t="shared" si="6"/>
-        <v>-1.6291903583263996</v>
+        <v>-2.1883674928666674</v>
       </c>
       <c r="W21">
         <f t="shared" si="6"/>
-        <v>-0.81459517916319979</v>
+        <v>-1.0941837464333337</v>
       </c>
       <c r="X21">
         <f t="shared" si="6"/>
@@ -4203,27 +4248,27 @@
       </c>
       <c r="Z21">
         <f t="shared" si="7"/>
-        <v>0.19491894742080085</v>
+        <v>0.22001672139999773</v>
       </c>
       <c r="AA21">
         <f t="shared" ref="AA21:AA25" si="8">S21-C21</f>
-        <v>0.18379732916800151</v>
+        <v>0.21186935233333148</v>
       </c>
       <c r="AB21">
         <f t="shared" ref="AB21:AB25" si="9">T21-D21</f>
-        <v>0.16420690275200078</v>
+        <v>0.19241613266666491</v>
       </c>
       <c r="AC21">
         <f t="shared" ref="AC21:AC25" si="10">U21-E21</f>
-        <v>0.13608995936640023</v>
+        <v>0.16158002119999892</v>
       </c>
       <c r="AD21">
         <f t="shared" ref="AD21:AD25" si="11">V21-F21</f>
-        <v>9.9388594249600448E-2</v>
+        <v>0.11928371513333236</v>
       </c>
       <c r="AE21">
         <f t="shared" ref="AE21:AE25" si="12">W21-G21</f>
-        <v>5.4044706684800214E-2</v>
+        <v>6.5449650066666365E-2</v>
       </c>
       <c r="AF21">
         <f t="shared" ref="AF21:AF25" si="13">X21-H21</f>
@@ -4231,471 +4276,471 @@
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>27</v>
       </c>
       <c r="B22">
         <f t="shared" si="4"/>
-        <v>-5.9598892199952003</v>
+        <v>-7.9564462690999997</v>
       </c>
       <c r="C22">
         <f t="shared" si="4"/>
-        <v>-5.1341724225791996</v>
+        <v>-6.8541151535999996</v>
       </c>
       <c r="D22">
         <f t="shared" si="4"/>
-        <v>-4.2999868169999997</v>
+        <v>-5.7404781874999999</v>
       </c>
       <c r="E22">
         <f t="shared" si="4"/>
-        <v>-3.4572746944512001</v>
+        <v>-4.6154583296</v>
       </c>
       <c r="F22">
         <f t="shared" si="4"/>
-        <v>-2.6059781501711998</v>
+        <v>-3.4789782771</v>
       </c>
       <c r="G22">
         <f t="shared" si="4"/>
-        <v>-1.7460390834432</v>
+        <v>-2.3309604656</v>
       </c>
       <c r="H22">
         <f t="shared" si="4"/>
-        <v>-0.87739919759520002</v>
+        <v>-1.1713270691</v>
       </c>
       <c r="J22">
         <f t="shared" si="5"/>
-        <v>0.85141274571359993</v>
+        <v>1.1366351813</v>
       </c>
       <c r="K22">
         <f t="shared" si="5"/>
-        <v>0.85569540376319997</v>
+        <v>1.1423525256</v>
       </c>
       <c r="L22">
         <f t="shared" si="5"/>
-        <v>0.85999736339999999</v>
+        <v>1.1480956375</v>
       </c>
       <c r="M22">
         <f t="shared" si="5"/>
-        <v>0.8643186736127999</v>
+        <v>1.1538645824</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
-        <v>0.86865938339039994</v>
+        <v>1.1596594256999999</v>
       </c>
       <c r="O22">
         <f t="shared" si="5"/>
-        <v>0.8730195417215999</v>
+        <v>1.1654802328</v>
       </c>
       <c r="P22">
         <f t="shared" si="5"/>
-        <v>0.87739919759519991</v>
+        <v>1.1713270691</v>
       </c>
       <c r="R22">
         <f t="shared" si="6"/>
-        <v>-5.7021662541423987</v>
+        <v>-7.6592862250333358</v>
       </c>
       <c r="S22">
         <f t="shared" si="6"/>
-        <v>-4.8875710749791992</v>
+        <v>-6.5651024786000018</v>
       </c>
       <c r="T22">
         <f t="shared" si="6"/>
-        <v>-4.0729758958159987</v>
+        <v>-5.4709187321666688</v>
       </c>
       <c r="U22">
         <f t="shared" si="6"/>
-        <v>-3.2583807166527992</v>
+        <v>-4.3767349857333349</v>
       </c>
       <c r="V22">
         <f t="shared" si="6"/>
-        <v>-2.4437855374895996</v>
+        <v>-3.2825512393000009</v>
       </c>
       <c r="W22">
         <f t="shared" si="6"/>
-        <v>-1.6291903583263996</v>
+        <v>-2.1883674928666674</v>
       </c>
       <c r="X22">
         <f t="shared" si="6"/>
-        <v>-0.81459517916319979</v>
+        <v>-1.0941837464333337</v>
       </c>
       <c r="Z22">
         <f t="shared" si="7"/>
-        <v>0.25772296585280152</v>
+        <v>0.29716004406666396</v>
       </c>
       <c r="AA22">
         <f t="shared" si="8"/>
-        <v>0.24660134760000041</v>
+        <v>0.28901267499999772</v>
       </c>
       <c r="AB22">
         <f t="shared" si="9"/>
-        <v>0.22701092118400101</v>
+        <v>0.26955945533333114</v>
       </c>
       <c r="AC22">
         <f t="shared" si="10"/>
-        <v>0.1988939777984009</v>
+        <v>0.23872334386666516</v>
       </c>
       <c r="AD22">
         <f t="shared" si="11"/>
-        <v>0.16219261268160023</v>
+        <v>0.19642703779999904</v>
       </c>
       <c r="AE22">
         <f t="shared" si="12"/>
-        <v>0.11684872511680044</v>
+        <v>0.1425929727333326</v>
       </c>
       <c r="AF22">
         <f t="shared" si="13"/>
-        <v>6.280401843200023E-2</v>
+        <v>7.7143322666666236E-2</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>28</v>
       </c>
       <c r="B23">
         <f t="shared" si="4"/>
-        <v>-6.8461064179199997</v>
+        <v>-9.1395453599999996</v>
       </c>
       <c r="C23">
         <f t="shared" si="4"/>
-        <v>-6.020389620504</v>
+        <v>-8.0372142444999994</v>
       </c>
       <c r="D23">
         <f t="shared" si="4"/>
-        <v>-5.1862040149248001</v>
+        <v>-6.9235772783999998</v>
       </c>
       <c r="E23">
         <f t="shared" si="4"/>
-        <v>-4.343491892376</v>
+        <v>-5.7985574204999999</v>
       </c>
       <c r="F23">
         <f t="shared" si="4"/>
-        <v>-3.4921953480959997</v>
+        <v>-4.6620773680000003</v>
       </c>
       <c r="G23">
         <f t="shared" si="4"/>
-        <v>-2.6322562813679999</v>
+        <v>-3.5140595564999999</v>
       </c>
       <c r="H23">
         <f t="shared" si="4"/>
-        <v>-1.7636163955199999</v>
+        <v>-2.35442616</v>
       </c>
       <c r="J23">
         <f t="shared" si="5"/>
-        <v>0.85576330223999997</v>
+        <v>1.14244317</v>
       </c>
       <c r="K23">
         <f t="shared" si="5"/>
-        <v>0.86005566007199996</v>
+        <v>1.1481734635</v>
       </c>
       <c r="L23">
         <f t="shared" si="5"/>
-        <v>0.86436733582079994</v>
+        <v>1.1539295464000001</v>
       </c>
       <c r="M23">
         <f t="shared" si="5"/>
-        <v>0.86869837847519993</v>
+        <v>1.1597114841</v>
       </c>
       <c r="N23">
         <f t="shared" si="5"/>
-        <v>0.87304883702400005</v>
+        <v>1.1655193419999998</v>
       </c>
       <c r="O23">
         <f t="shared" si="5"/>
-        <v>0.87741876045599998</v>
+        <v>1.1713531854999999</v>
       </c>
       <c r="P23">
         <f t="shared" si="5"/>
-        <v>0.88180819775999997</v>
+        <v>1.1772130799999998</v>
       </c>
       <c r="R23">
         <f t="shared" si="6"/>
-        <v>-6.5167614333055983</v>
+        <v>-8.7534699714666697</v>
       </c>
       <c r="S23">
         <f t="shared" si="6"/>
-        <v>-5.7021662541423987</v>
+        <v>-7.6592862250333358</v>
       </c>
       <c r="T23">
         <f t="shared" si="6"/>
-        <v>-4.8875710749791992</v>
+        <v>-6.5651024786000018</v>
       </c>
       <c r="U23">
         <f t="shared" si="6"/>
-        <v>-4.0729758958159987</v>
+        <v>-5.4709187321666688</v>
       </c>
       <c r="V23">
         <f t="shared" si="6"/>
-        <v>-3.2583807166527992</v>
+        <v>-4.3767349857333349</v>
       </c>
       <c r="W23">
         <f t="shared" si="6"/>
-        <v>-2.4437855374895996</v>
+        <v>-3.2825512393000009</v>
       </c>
       <c r="X23">
         <f t="shared" si="6"/>
-        <v>-1.6291903583263996</v>
+        <v>-2.1883674928666674</v>
       </c>
       <c r="Z23">
         <f t="shared" si="7"/>
-        <v>0.32934498461440143</v>
+        <v>0.3860753885333299</v>
       </c>
       <c r="AA23">
         <f t="shared" si="8"/>
-        <v>0.3182233663616012</v>
+        <v>0.37792801946666366</v>
       </c>
       <c r="AB23">
         <f t="shared" si="9"/>
-        <v>0.29863293994560092</v>
+        <v>0.35847479979999797</v>
       </c>
       <c r="AC23">
         <f t="shared" si="10"/>
-        <v>0.27051599656000125</v>
+        <v>0.3276386883333311</v>
       </c>
       <c r="AD23">
         <f t="shared" si="11"/>
-        <v>0.23381463144320058</v>
+        <v>0.28534238226666542</v>
       </c>
       <c r="AE23">
         <f t="shared" si="12"/>
-        <v>0.18847074387840035</v>
+        <v>0.23150831719999898</v>
       </c>
       <c r="AF23">
         <f t="shared" si="13"/>
-        <v>0.13442603719360036</v>
+        <v>0.16605866713333262</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>29</v>
       </c>
       <c r="B24">
         <f t="shared" si="4"/>
-        <v>-7.7412005007119999</v>
+        <v>-10.3344950835</v>
       </c>
       <c r="C24">
         <f t="shared" si="4"/>
-        <v>-6.9154837032960002</v>
+        <v>-9.2321639680000001</v>
       </c>
       <c r="D24">
         <f t="shared" si="4"/>
-        <v>-6.0812980977167994</v>
+        <v>-8.1185270019000004</v>
       </c>
       <c r="E24">
         <f t="shared" si="4"/>
-        <v>-5.2385859751680002</v>
+        <v>-6.9935071439999996</v>
       </c>
       <c r="F24">
         <f t="shared" si="4"/>
-        <v>-4.3872894308879999</v>
+        <v>-5.8570270915</v>
       </c>
       <c r="G24">
         <f t="shared" si="4"/>
-        <v>-3.5273503641599997</v>
+        <v>-4.7090092800000001</v>
       </c>
       <c r="H24">
         <f t="shared" si="4"/>
-        <v>-2.6587104783119999</v>
+        <v>-3.5493758835000002</v>
       </c>
       <c r="J24">
         <f t="shared" si="5"/>
-        <v>0.86013338896799996</v>
+        <v>1.1482772315000001</v>
       </c>
       <c r="K24">
         <f t="shared" si="5"/>
-        <v>0.86443546291199991</v>
+        <v>1.154020496</v>
       </c>
       <c r="L24">
         <f t="shared" si="5"/>
-        <v>0.86875687110239996</v>
+        <v>1.1597895717</v>
       </c>
       <c r="M24">
         <f t="shared" si="5"/>
-        <v>0.87309766252799992</v>
+        <v>1.165584524</v>
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
-        <v>0.8774578861775999</v>
+        <v>1.1714054183000002</v>
       </c>
       <c r="O24">
         <f t="shared" si="5"/>
-        <v>0.88183759103999992</v>
+        <v>1.17725232</v>
       </c>
       <c r="P24">
         <f t="shared" si="5"/>
-        <v>0.8862368261039999</v>
+        <v>1.1831252944999999</v>
       </c>
       <c r="R24">
         <f t="shared" si="6"/>
-        <v>-7.3313566124687979</v>
+        <v>-9.8476537179000037</v>
       </c>
       <c r="S24">
         <f t="shared" si="6"/>
-        <v>-6.5167614333055983</v>
+        <v>-8.7534699714666697</v>
       </c>
       <c r="T24">
         <f t="shared" si="6"/>
-        <v>-5.7021662541423987</v>
+        <v>-7.6592862250333358</v>
       </c>
       <c r="U24">
         <f t="shared" si="6"/>
-        <v>-4.8875710749791992</v>
+        <v>-6.5651024786000018</v>
       </c>
       <c r="V24">
         <f t="shared" si="6"/>
-        <v>-4.0729758958159987</v>
+        <v>-5.4709187321666688</v>
       </c>
       <c r="W24">
         <f t="shared" si="6"/>
-        <v>-3.2583807166527992</v>
+        <v>-4.3767349857333349</v>
       </c>
       <c r="X24">
         <f t="shared" si="6"/>
-        <v>-2.4437855374895996</v>
+        <v>-3.2825512393000009</v>
       </c>
       <c r="Z24">
         <f t="shared" si="7"/>
-        <v>0.40984388824320206</v>
+        <v>0.48684136559999658</v>
       </c>
       <c r="AA24">
         <f t="shared" si="8"/>
-        <v>0.39872226999040183</v>
+        <v>0.47869399653333033</v>
       </c>
       <c r="AB24">
         <f t="shared" si="9"/>
-        <v>0.37913184357440066</v>
+        <v>0.45924077686666465</v>
       </c>
       <c r="AC24">
         <f t="shared" si="10"/>
-        <v>0.35101490018880099</v>
+        <v>0.42840466539999777</v>
       </c>
       <c r="AD24">
         <f t="shared" si="11"/>
-        <v>0.31431353507200122</v>
+        <v>0.38610835933333121</v>
       </c>
       <c r="AE24">
         <f t="shared" si="12"/>
-        <v>0.26896964750720054</v>
+        <v>0.33227429426666522</v>
       </c>
       <c r="AF24">
         <f t="shared" si="13"/>
-        <v>0.21492494082240032</v>
+        <v>0.26682464419999929</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>30</v>
       </c>
       <c r="B25">
         <f t="shared" si="4"/>
-        <v>-8.6452305488639993</v>
+        <v>-11.541374312</v>
       </c>
       <c r="C25">
         <f t="shared" si="4"/>
-        <v>-7.8195137514479995</v>
+        <v>-10.4390431965</v>
       </c>
       <c r="D25">
         <f t="shared" si="4"/>
-        <v>-6.9853281458687997</v>
+        <v>-9.3254062304000005</v>
       </c>
       <c r="E25">
         <f t="shared" si="4"/>
-        <v>-6.1426160233199996</v>
+        <v>-8.2003863725000006</v>
       </c>
       <c r="F25">
         <f t="shared" si="4"/>
-        <v>-5.2913194790400002</v>
+        <v>-7.0639063200000001</v>
       </c>
       <c r="G25">
         <f t="shared" si="4"/>
-        <v>-4.4313804123119995</v>
+        <v>-5.9158885085000001</v>
       </c>
       <c r="H25">
         <f t="shared" si="4"/>
-        <v>-3.5627405264639997</v>
+        <v>-4.7562551119999998</v>
       </c>
       <c r="J25">
         <f t="shared" si="5"/>
-        <v>0.86452305488640002</v>
+        <v>1.1541374311999999</v>
       </c>
       <c r="K25">
         <f t="shared" si="5"/>
-        <v>0.86883486127199994</v>
+        <v>1.1598936885</v>
       </c>
       <c r="L25">
         <f t="shared" si="5"/>
-        <v>0.87316601823359996</v>
+        <v>1.1656757788000001</v>
       </c>
       <c r="M25">
         <f t="shared" si="5"/>
-        <v>0.87751657475999989</v>
+        <v>1.1714837675000001</v>
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
-        <v>0.88188657983999996</v>
+        <v>1.17731772</v>
       </c>
       <c r="O25">
         <f t="shared" si="5"/>
-        <v>0.88627608246239997</v>
+        <v>1.1831777017</v>
       </c>
       <c r="P25">
         <f t="shared" si="5"/>
-        <v>0.89068513161599994</v>
+        <v>1.189063778</v>
       </c>
       <c r="R25">
         <f t="shared" si="6"/>
-        <v>-8.1459517916319975</v>
+        <v>-10.941837464333338</v>
       </c>
       <c r="S25">
         <f t="shared" si="6"/>
-        <v>-7.3313566124687979</v>
+        <v>-9.8476537179000037</v>
       </c>
       <c r="T25">
         <f t="shared" si="6"/>
-        <v>-6.5167614333055983</v>
+        <v>-8.7534699714666697</v>
       </c>
       <c r="U25">
         <f t="shared" si="6"/>
-        <v>-5.7021662541423987</v>
+        <v>-7.6592862250333358</v>
       </c>
       <c r="V25">
         <f t="shared" si="6"/>
-        <v>-4.8875710749791992</v>
+        <v>-6.5651024786000018</v>
       </c>
       <c r="W25">
         <f t="shared" si="6"/>
-        <v>-4.0729758958159987</v>
+        <v>-5.4709187321666688</v>
       </c>
       <c r="X25">
         <f t="shared" si="6"/>
-        <v>-3.2583807166527992</v>
+        <v>-4.3767349857333349</v>
       </c>
       <c r="Z25">
         <f t="shared" si="7"/>
-        <v>0.49927875723200188</v>
+        <v>0.59953684766666271</v>
       </c>
       <c r="AA25">
         <f t="shared" si="8"/>
-        <v>0.48815713897920165</v>
+        <v>0.59138947859999647</v>
       </c>
       <c r="AB25">
         <f t="shared" si="9"/>
-        <v>0.46856671256320137</v>
+        <v>0.57193625893333078</v>
       </c>
       <c r="AC25">
         <f t="shared" si="10"/>
-        <v>0.44044976917760081</v>
+        <v>0.54110014746666479</v>
       </c>
       <c r="AD25">
         <f t="shared" si="11"/>
-        <v>0.40374840406080104</v>
+        <v>0.49880384139999823</v>
       </c>
       <c r="AE25">
         <f t="shared" si="12"/>
-        <v>0.3584045164960008</v>
+        <v>0.44496977633333135</v>
       </c>
       <c r="AF25">
         <f t="shared" si="13"/>
-        <v>0.30435980981120059</v>
+        <v>0.37952012626666498</v>
       </c>
     </row>
   </sheetData>
@@ -4712,16 +4757,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
In pprojector3, debugging KT -> PT
</commit_message>
<xml_diff>
--- a/doc/Aquarium.xlsx
+++ b/doc/Aquarium.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="8595" windowHeight="8940"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="8595" windowHeight="8940" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="thermistor" sheetId="3" r:id="rId1"/>
@@ -12,21 +12,21 @@
     <sheet name="scratch" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="a">thermistor!$B$1</definedName>
-    <definedName name="b">thermistor!$B$2</definedName>
-    <definedName name="Rref">thermistor!$B$9</definedName>
-    <definedName name="SH_c">thermistor!$B$3</definedName>
-    <definedName name="T">thermistor!$B$4</definedName>
-    <definedName name="Vref">thermistor!$B$8</definedName>
-    <definedName name="x">thermistor!$B$6</definedName>
-    <definedName name="y">thermistor!$B$5</definedName>
+    <definedName name="a">thermistor!$B$2</definedName>
+    <definedName name="b">thermistor!$B$3</definedName>
+    <definedName name="Rref">thermistor!$B$10</definedName>
+    <definedName name="SH_c">thermistor!$B$4</definedName>
+    <definedName name="T">thermistor!$B$5</definedName>
+    <definedName name="Vref">thermistor!$B$9</definedName>
+    <definedName name="x">thermistor!$B$7</definedName>
+    <definedName name="y">thermistor!$B$6</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>T_air</t>
   </si>
@@ -108,6 +108,27 @@
   <si>
     <t>Trange</t>
   </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>QTRL2Z-103C3-12</t>
+  </si>
+  <si>
+    <t>Rtot =</t>
+  </si>
+  <si>
+    <t>Amp</t>
+  </si>
+  <si>
+    <t>Power =</t>
+  </si>
+  <si>
+    <t>Current =</t>
+  </si>
+  <si>
+    <t>Watt</t>
+  </si>
 </sst>
 </file>
 
@@ -163,21 +184,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,12 +807,12 @@
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="132050304"/>
-        <c:axId val="132457984"/>
-        <c:axId val="132016320"/>
+        <c:axId val="96950912"/>
+        <c:axId val="96957184"/>
+        <c:axId val="40757888"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="132050304"/>
+        <c:axId val="96950912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -825,7 +847,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="132457984"/>
+        <c:crossAx val="96957184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -833,7 +855,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132457984"/>
+        <c:axId val="96957184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,12 +892,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132050304"/>
+        <c:crossAx val="96950912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="132016320"/>
+        <c:axId val="40757888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -910,7 +932,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="132457984"/>
+        <c:crossAx val="96957184"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -1519,12 +1541,12 @@
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="132510080"/>
-        <c:axId val="132512000"/>
-        <c:axId val="132462784"/>
+        <c:axId val="104938880"/>
+        <c:axId val="104945152"/>
+        <c:axId val="96955008"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="132510080"/>
+        <c:axId val="104938880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1581,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="132512000"/>
+        <c:crossAx val="104945152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1567,7 +1589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132512000"/>
+        <c:axId val="104945152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -1606,12 +1628,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132510080"/>
+        <c:crossAx val="104938880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="132462784"/>
+        <c:axId val="96955008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1646,7 +1668,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="132512000"/>
+        <c:crossAx val="104945152"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -2014,10 +2036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2026,161 +2048,199 @@
     <col min="3" max="3" width="5.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7">
-        <v>1.4E-3</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B2" s="5">
+        <v>1.1127534437700001E-3</v>
+      </c>
+      <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="E1">
+      <c r="E2">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7">
-        <v>2.3699999999999999E-4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" s="5">
+        <v>2.36732362183E-4</v>
+      </c>
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7">
-        <v>9.9E-8</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B4" s="5">
+        <v>7.8005993000000005E-8</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="E3">
-        <f>E1-E2</f>
+      <c r="E4">
+        <f>E2-E3</f>
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="8">
-        <f>10+273</f>
-        <v>283</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B5" s="6">
+        <f>37+273</f>
+        <v>310</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B6" s="6">
         <f>(a - 1/T) / SH_c</f>
-        <v>-21551.201056501406</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <v>-27088.341889871244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <f>SQRT((b/(3*SH_c))^3 + y^2/4)</f>
-        <v>24984.886742582079</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>34909.122745868546</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <f xml:space="preserve"> EXP( (x - y/2)^(1/3) - (x+y/2)^(1/3) )</f>
-        <v>6154.6038555506448</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+        <v>6052.9970389552454</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <f>B8+Rref</f>
+        <v>16052.997038955245</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B9" s="7">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1">
+        <f>Vref/E8</f>
+        <v>3.114683188358333E-4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B10" s="7">
         <v>10000</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="1">
+        <f>E9^2 * B8</f>
+        <v>5.872164577949635E-4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
-        <f xml:space="preserve"> B7* Vref / (Rref + B7)</f>
-        <v>1.9049070811587721</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11">
-        <f>1.9-0.78</f>
-        <v>1.1199999999999999</v>
+        <f xml:space="preserve"> B8* Vref / (Rref + B8)</f>
+        <v>1.8853168116416672</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" t="s">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f>3.34-1.89</f>
+        <v>1.45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B12">
+      <c r="B14">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <f>B12 + LOG(B11/Vref) / LOG(2)</f>
-        <v>9.8415706373955167</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f>B14 + LOG(B13/Vref) / LOG(2)</f>
+        <v>10.214124805352848</v>
+      </c>
+      <c r="C15" t="s">
         <v>22</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <f>E3/2^B13</f>
-        <v>2.942766462053574E-2</v>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>E4/2^B15</f>
+        <v>2.2730334051724154E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2230,81 +2290,81 @@
       </c>
     </row>
     <row r="2" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="J2" s="5" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="J2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="R2" s="5" t="s">
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="R2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Z2" s="5" t="s">
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Z2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
     </row>
     <row r="3" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="J3" s="6" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="J3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="R3" s="6" t="s">
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="R3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Z3" s="6" t="s">
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Z3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
     </row>
     <row r="4" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -4872,131 +4932,128 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>32.450000000000003</v>
+        <v>45.57</v>
       </c>
       <c r="B1">
+        <v>10.37</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2618</v>
+      </c>
+      <c r="D1">
         <v>31.36</v>
       </c>
-      <c r="C1" s="1">
-        <v>1.0940000000000001</v>
+      <c r="E1" s="10">
+        <v>51002</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2184</v>
+        <v>48384</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <f>A1/A2</f>
-        <v>1.4858058608058609E-2</v>
-      </c>
-      <c r="B3">
+        <v>9.4184027777777777E-4</v>
+      </c>
+      <c r="B3" s="1">
         <f>B1/A2</f>
-        <v>1.4358974358974359E-2</v>
+        <v>2.1432705026455025E-4</v>
       </c>
       <c r="C3" s="1">
         <f>C1/A2</f>
-        <v>5.0091575091575091E-4</v>
+        <v>5.4108796296296294E-2</v>
+      </c>
+      <c r="D3" s="1">
+        <f>D1/A2</f>
+        <v>6.4814814814814813E-4</v>
+      </c>
+      <c r="E3" s="1">
+        <f>E1/A2</f>
+        <v>1.0541087962962963</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="1"/>
+      <c r="A5">
+        <v>32.450000000000003</v>
+      </c>
+      <c r="B5">
+        <v>31.36</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2184</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>2184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f>A5/A6</f>
+        <v>1.4858058608058609E-2</v>
+      </c>
+      <c r="B7" s="1">
+        <f>B5/A6</f>
+        <v>1.4358974358974359E-2</v>
+      </c>
+      <c r="C7" s="1">
+        <f>C5/A6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>10.37</v>
       </c>
-      <c r="B6">
-        <v>45.57</v>
-      </c>
-      <c r="C6">
-        <v>31.36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>48384</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f>A6/A7</f>
-        <v>2.1432705026455025E-4</v>
-      </c>
-      <c r="B8">
-        <f>B6/A7</f>
-        <v>9.4184027777777777E-4</v>
-      </c>
-      <c r="C8">
-        <f>C6/A7</f>
-        <v>6.4814814814814813E-4</v>
+      <c r="B9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>2.14E-4</v>
-      </c>
-      <c r="B10" s="4">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C10" s="1">
-        <f>A10*B10</f>
-        <v>8.5600000000000004E-7</v>
-      </c>
-      <c r="D10" s="4">
-        <v>3.8200000000000002E-4</v>
-      </c>
-      <c r="E10" s="1">
-        <f>B10*D10</f>
-        <v>1.528E-6</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1.15E-2</v>
-      </c>
-      <c r="G10" s="1">
-        <f>E10*F10</f>
-        <v>1.7572E-8</v>
-      </c>
+        <v>2618</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>6.4800000000000003E-4</v>
+        <f>A9/A10</f>
+        <v>3.9610389610389611E-3</v>
       </c>
       <c r="B11" s="4">
-        <v>1.14E-2</v>
-      </c>
-      <c r="C11" s="1">
-        <f>A11*B11</f>
-        <v>7.3872000000000002E-6</v>
-      </c>
-      <c r="D11" s="4">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="E11" s="1">
-        <f>B11*D11</f>
-        <v>5.7000000000000005E-6</v>
-      </c>
-      <c r="F11" s="1">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="G11" s="1">
-        <f>E11*F11</f>
-        <v>2.2800000000000002E-8</v>
-      </c>
+        <f>B9/A10</f>
+        <v>3.8197097020626432E-4</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>

</xml_diff>